<commit_message>
Fix: Update top_jobs_by_type.py to use PerformanceOptimizer for accurate speed and flight hour calculations
- Import PerformanceOptimizer and initialize in main()
- Replace static speed lookup with per-leg optimized speed calculations
- Calculate flight hours using optimized speeds per leg for aircraft with performance curves
- Fallback to original method for aircraft without sample data
- CSV now shows realistic variable speeds within observed ranges instead of static database values
- Fixes issue where CSV speeds didn't match the implemented performance optimizations
</commit_message>
<xml_diff>
--- a/planes.xlsx
+++ b/planes.xlsx
@@ -8,20 +8,33 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aaron\OnAir\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{525BC214-B92B-468F-B49A-7D1AF16058C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AAE1AC1-93E6-4847-925D-90151EA0802C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{7DA1CCB9-1292-47D3-ABC3-3EB19435A409}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{7DA1CCB9-1292-47D3-ABC3-3EB19435A409}"/>
   </bookViews>
   <sheets>
     <sheet name="Planes" sheetId="1" r:id="rId1"/>
     <sheet name="Jobs" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="55">
   <si>
     <t>Plane</t>
   </si>
@@ -123,9 +136,6 @@
   </si>
   <si>
     <t>KGYR</t>
-  </si>
-  <si>
-    <t>KFJK</t>
   </si>
   <si>
     <t>LFRC</t>
@@ -1051,7 +1061,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A16643A-B77F-44B3-83CF-168AF5426912}">
   <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
@@ -1306,8 +1316,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B22E5411-C937-41B5-8075-5A67875F9274}">
   <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1501,10 +1511,10 @@
         <v>8</v>
       </c>
       <c r="B7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" t="s">
         <v>34</v>
-      </c>
-      <c r="C7" t="s">
-        <v>35</v>
       </c>
       <c r="D7">
         <v>2987</v>
@@ -1530,10 +1540,10 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" t="s">
         <v>35</v>
-      </c>
-      <c r="C8" t="s">
-        <v>36</v>
       </c>
       <c r="D8">
         <v>1441</v>
@@ -1559,10 +1569,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" t="s">
         <v>36</v>
-      </c>
-      <c r="C9" t="s">
-        <v>37</v>
       </c>
       <c r="D9">
         <v>1183</v>
@@ -1588,10 +1598,10 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" t="s">
         <v>37</v>
-      </c>
-      <c r="C10" t="s">
-        <v>38</v>
       </c>
       <c r="D10">
         <v>3186</v>
@@ -1617,10 +1627,10 @@
         <v>12</v>
       </c>
       <c r="B11" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" t="s">
         <v>39</v>
-      </c>
-      <c r="C11" t="s">
-        <v>40</v>
       </c>
       <c r="D11">
         <v>3931</v>
@@ -1646,10 +1656,10 @@
         <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D12">
         <v>3931</v>
@@ -1675,10 +1685,10 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D13">
         <v>4759</v>
@@ -1704,10 +1714,10 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D14">
         <v>4759</v>
@@ -1733,10 +1743,10 @@
         <v>12</v>
       </c>
       <c r="B15" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15" t="s">
         <v>39</v>
-      </c>
-      <c r="C15" t="s">
-        <v>40</v>
       </c>
       <c r="D15">
         <v>3931</v>
@@ -1762,10 +1772,10 @@
         <v>12</v>
       </c>
       <c r="B16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D16">
         <v>3931</v>
@@ -1791,10 +1801,10 @@
         <v>12</v>
       </c>
       <c r="B17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C17" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D17">
         <v>4759</v>
@@ -1820,10 +1830,10 @@
         <v>12</v>
       </c>
       <c r="B18" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D18">
         <v>4759</v>
@@ -1849,10 +1859,10 @@
         <v>13</v>
       </c>
       <c r="B19" t="s">
+        <v>41</v>
+      </c>
+      <c r="C19" t="s">
         <v>42</v>
-      </c>
-      <c r="C19" t="s">
-        <v>43</v>
       </c>
       <c r="D19">
         <v>1983</v>
@@ -1878,10 +1888,10 @@
         <v>13</v>
       </c>
       <c r="B20" t="s">
+        <v>42</v>
+      </c>
+      <c r="C20" t="s">
         <v>43</v>
-      </c>
-      <c r="C20" t="s">
-        <v>44</v>
       </c>
       <c r="D20">
         <v>1548</v>
@@ -1907,10 +1917,10 @@
         <v>13</v>
       </c>
       <c r="B21" t="s">
+        <v>43</v>
+      </c>
+      <c r="C21" t="s">
         <v>44</v>
-      </c>
-      <c r="C21" t="s">
-        <v>45</v>
       </c>
       <c r="D21">
         <v>415</v>
@@ -1936,10 +1946,10 @@
         <v>13</v>
       </c>
       <c r="B22" t="s">
+        <v>44</v>
+      </c>
+      <c r="C22" t="s">
         <v>45</v>
-      </c>
-      <c r="C22" t="s">
-        <v>46</v>
       </c>
       <c r="D22">
         <v>1954</v>
@@ -1965,10 +1975,10 @@
         <v>13</v>
       </c>
       <c r="B23" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D23">
         <v>3037</v>
@@ -1994,10 +2004,10 @@
         <v>13</v>
       </c>
       <c r="B24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C24" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D24">
         <v>2727</v>
@@ -2023,10 +2033,10 @@
         <v>13</v>
       </c>
       <c r="B25" t="s">
+        <v>46</v>
+      </c>
+      <c r="C25" t="s">
         <v>47</v>
-      </c>
-      <c r="C25" t="s">
-        <v>48</v>
       </c>
       <c r="D25">
         <v>2034</v>
@@ -2052,10 +2062,10 @@
         <v>13</v>
       </c>
       <c r="B26" t="s">
+        <v>47</v>
+      </c>
+      <c r="C26" t="s">
         <v>48</v>
-      </c>
-      <c r="C26" t="s">
-        <v>49</v>
       </c>
       <c r="D26">
         <v>1100</v>
@@ -2081,10 +2091,10 @@
         <v>13</v>
       </c>
       <c r="B27" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C27" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D27">
         <v>226</v>
@@ -2110,10 +2120,10 @@
         <v>16</v>
       </c>
       <c r="B28" t="s">
+        <v>49</v>
+      </c>
+      <c r="C28" t="s">
         <v>50</v>
-      </c>
-      <c r="C28" t="s">
-        <v>51</v>
       </c>
       <c r="D28">
         <v>306</v>
@@ -2139,10 +2149,10 @@
         <v>16</v>
       </c>
       <c r="B29" t="s">
+        <v>50</v>
+      </c>
+      <c r="C29" t="s">
         <v>51</v>
-      </c>
-      <c r="C29" t="s">
-        <v>52</v>
       </c>
       <c r="D29">
         <v>1084</v>
@@ -2168,10 +2178,10 @@
         <v>16</v>
       </c>
       <c r="B30" t="s">
+        <v>51</v>
+      </c>
+      <c r="C30" t="s">
         <v>52</v>
-      </c>
-      <c r="C30" t="s">
-        <v>53</v>
       </c>
       <c r="D30">
         <v>959</v>
@@ -2197,10 +2207,10 @@
         <v>16</v>
       </c>
       <c r="B31" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C31" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D31">
         <v>1716</v>
@@ -2226,10 +2236,10 @@
         <v>16</v>
       </c>
       <c r="B32" t="s">
+        <v>53</v>
+      </c>
+      <c r="C32" t="s">
         <v>54</v>
-      </c>
-      <c r="C32" t="s">
-        <v>55</v>
       </c>
       <c r="D32">
         <v>528</v>
@@ -2255,10 +2265,10 @@
         <v>16</v>
       </c>
       <c r="B33" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C33" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D33">
         <v>1678</v>

</xml_diff>

<commit_message>
Fix work order calculation issues
- Fix transit legs: calculate actual distance using Haversine formula instead of 0nm
- Fix transit legs: calculate realistic flight hours based on distance/speed instead of hardcoded 1.00h
- Fix transit legs: use proper aircraft speed from API data instead of 0 kts
- Fix transit legs: count as 0 legs instead of 1 leg in work orders
- Fix flight hours calculation: handle planes not in planes.xlsx by falling back to API speed data
- Fix speed lookup: when optimizer returns 0 (no performance curves), fall back to base speed
- Add _calculate_distance_between_airports() method for accurate airport-to-airport distances
- Improve error handling and fallback logic for speed calculations
- All work orders now show realistic distances, speeds, and flight hours
</commit_message>
<xml_diff>
--- a/planes.xlsx
+++ b/planes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aaron\OnAir\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AAE1AC1-93E6-4847-925D-90151EA0802C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFE2E665-1D86-465F-86B8-72D618E9A4D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{7DA1CCB9-1292-47D3-ABC3-3EB19435A409}"/>
+    <workbookView xWindow="30630" yWindow="3390" windowWidth="21600" windowHeight="12645" activeTab="1" xr2:uid="{7DA1CCB9-1292-47D3-ABC3-3EB19435A409}"/>
   </bookViews>
   <sheets>
     <sheet name="Planes" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="65">
   <si>
     <t>Plane</t>
   </si>
@@ -199,6 +199,36 @@
   </si>
   <si>
     <t>MKJS</t>
+  </si>
+  <si>
+    <t>KJER</t>
+  </si>
+  <si>
+    <t>KEMM</t>
+  </si>
+  <si>
+    <t>KUKF</t>
+  </si>
+  <si>
+    <t>KRPH</t>
+  </si>
+  <si>
+    <t>KGAG</t>
+  </si>
+  <si>
+    <t>KUKI</t>
+  </si>
+  <si>
+    <t>X35</t>
+  </si>
+  <si>
+    <t>PANC</t>
+  </si>
+  <si>
+    <t>KSDF</t>
+  </si>
+  <si>
+    <t>KCVG</t>
   </si>
 </sst>
 </file>
@@ -1314,10 +1344,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B22E5411-C937-41B5-8075-5A67875F9274}">
-  <dimension ref="A1:I33"/>
+  <dimension ref="A1:I53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A52" sqref="A52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1624,234 +1655,234 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B11" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C11" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="D11">
-        <v>3931</v>
+        <v>1983</v>
       </c>
       <c r="E11">
-        <v>6</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="F11">
-        <v>26678</v>
+        <v>21251</v>
       </c>
       <c r="G11">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H11">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I11">
-        <v>47765</v>
+        <v>12106</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B12" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="C12" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="D12">
-        <v>3931</v>
+        <v>1548</v>
       </c>
       <c r="E12">
-        <v>6</v>
+        <v>1.8</v>
       </c>
       <c r="F12">
-        <v>26542</v>
+        <v>17679</v>
       </c>
       <c r="G12">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H12">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I12">
-        <v>46553</v>
+        <v>3318</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="C13" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="D13">
-        <v>4759</v>
+        <v>415</v>
       </c>
       <c r="E13">
-        <v>7.1</v>
+        <v>0.9</v>
       </c>
       <c r="F13">
-        <v>31912</v>
+        <v>8443</v>
       </c>
       <c r="G13">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H13">
         <v>4</v>
       </c>
       <c r="I13">
-        <v>40982</v>
+        <v>25201</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="C14" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="D14">
-        <v>4759</v>
+        <v>1954</v>
       </c>
       <c r="E14">
-        <v>7.1</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="F14">
-        <v>31601</v>
+        <v>20857</v>
       </c>
       <c r="G14">
         <v>4</v>
       </c>
       <c r="H14">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I14">
-        <v>37607</v>
+        <v>22586</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="C15" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D15">
-        <v>3931</v>
+        <v>3037</v>
       </c>
       <c r="E15">
-        <v>6</v>
+        <v>3.1</v>
       </c>
       <c r="F15">
-        <v>26678</v>
+        <v>30551</v>
       </c>
       <c r="G15">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H15">
         <v>5</v>
       </c>
       <c r="I15">
-        <v>47765</v>
+        <v>19837</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B16" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C16" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="D16">
-        <v>3931</v>
+        <v>2727</v>
       </c>
       <c r="E16">
-        <v>6</v>
+        <v>2.8</v>
       </c>
       <c r="F16">
-        <v>26542</v>
+        <v>27806</v>
       </c>
       <c r="G16">
         <v>5</v>
       </c>
       <c r="H16">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I16">
-        <v>46553</v>
+        <v>9758</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B17" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="C17" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="D17">
-        <v>4759</v>
+        <v>2034</v>
       </c>
       <c r="E17">
-        <v>7.1</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="F17">
-        <v>31912</v>
+        <v>24970</v>
       </c>
       <c r="G17">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H17">
         <v>4</v>
       </c>
       <c r="I17">
-        <v>40982</v>
+        <v>14131</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B18" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="C18" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="D18">
-        <v>4759</v>
+        <v>1100</v>
       </c>
       <c r="E18">
-        <v>7.1</v>
+        <v>1.4</v>
       </c>
       <c r="F18">
-        <v>31601</v>
+        <v>14081</v>
       </c>
       <c r="G18">
         <v>4</v>
       </c>
       <c r="H18">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="I18">
-        <v>37607</v>
+        <v>27903</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -1859,164 +1890,164 @@
         <v>13</v>
       </c>
       <c r="B19" t="s">
+        <v>48</v>
+      </c>
+      <c r="C19" t="s">
         <v>41</v>
       </c>
-      <c r="C19" t="s">
-        <v>42</v>
-      </c>
       <c r="D19">
-        <v>1983</v>
+        <v>226</v>
       </c>
       <c r="E19">
-        <v>2.2000000000000002</v>
+        <v>0.7</v>
       </c>
       <c r="F19">
-        <v>21251</v>
+        <v>7917</v>
       </c>
       <c r="G19">
         <v>5</v>
       </c>
       <c r="H19">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I19">
-        <v>12106</v>
+        <v>31131</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B20" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="C20" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="D20">
-        <v>1548</v>
+        <v>306</v>
       </c>
       <c r="E20">
-        <v>1.8</v>
+        <v>0.7</v>
       </c>
       <c r="F20">
-        <v>17679</v>
+        <v>6179</v>
       </c>
       <c r="G20">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H20">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I20">
-        <v>3318</v>
+        <v>61</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B21" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="C21" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="D21">
-        <v>415</v>
+        <v>1084</v>
       </c>
       <c r="E21">
-        <v>0.9</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="F21">
-        <v>8443</v>
+        <v>10949</v>
       </c>
       <c r="G21">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H21">
         <v>4</v>
       </c>
       <c r="I21">
-        <v>25201</v>
+        <v>56</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B22" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="C22" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="D22">
-        <v>1954</v>
+        <v>959</v>
       </c>
       <c r="E22">
-        <v>2.2000000000000002</v>
+        <v>1</v>
       </c>
       <c r="F22">
-        <v>20857</v>
+        <v>11546</v>
       </c>
       <c r="G22">
         <v>4</v>
       </c>
       <c r="H22">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I22">
-        <v>22586</v>
+        <v>31</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B23" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="C23" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="D23">
-        <v>3037</v>
+        <v>1716</v>
       </c>
       <c r="E23">
-        <v>3.1</v>
+        <v>1.4</v>
       </c>
       <c r="F23">
-        <v>30551</v>
+        <v>11721</v>
       </c>
       <c r="G23">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H23">
         <v>5</v>
       </c>
       <c r="I23">
-        <v>19837</v>
+        <v>52</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B24" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="C24" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="D24">
-        <v>2727</v>
+        <v>528</v>
       </c>
       <c r="E24">
-        <v>2.8</v>
+        <v>0.8</v>
       </c>
       <c r="F24">
-        <v>27806</v>
+        <v>6601</v>
       </c>
       <c r="G24">
         <v>5</v>
@@ -2025,271 +2056,854 @@
         <v>4</v>
       </c>
       <c r="I24">
-        <v>9758</v>
+        <v>67</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B25" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="C25" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D25">
-        <v>2034</v>
+        <v>1678</v>
       </c>
       <c r="E25">
-        <v>2.2000000000000002</v>
+        <v>1.4</v>
       </c>
       <c r="F25">
-        <v>24970</v>
+        <v>11520</v>
       </c>
       <c r="G25">
         <v>4</v>
       </c>
       <c r="H25">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I25">
-        <v>14131</v>
+        <v>51</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B26" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="C26" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="D26">
-        <v>1100</v>
+        <v>3931</v>
       </c>
       <c r="E26">
-        <v>1.4</v>
+        <v>6</v>
       </c>
       <c r="F26">
-        <v>14081</v>
+        <v>26678</v>
       </c>
       <c r="G26">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H26">
         <v>5</v>
       </c>
       <c r="I26">
-        <v>27903</v>
+        <v>47765</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B27" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="C27" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D27">
-        <v>226</v>
+        <v>3931</v>
       </c>
       <c r="E27">
-        <v>0.7</v>
+        <v>6</v>
       </c>
       <c r="F27">
-        <v>7917</v>
+        <v>26542</v>
       </c>
       <c r="G27">
         <v>5</v>
       </c>
       <c r="H27">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="I27">
-        <v>31131</v>
+        <v>46553</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B28" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="C28" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="D28">
-        <v>306</v>
+        <v>4759</v>
       </c>
       <c r="E28">
-        <v>0.7</v>
+        <v>7.1</v>
       </c>
       <c r="F28">
-        <v>6179</v>
+        <v>31912</v>
       </c>
       <c r="G28">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H28">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I28">
-        <v>61</v>
+        <v>40982</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B29" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="C29" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="D29">
-        <v>1084</v>
+        <v>4759</v>
       </c>
       <c r="E29">
-        <v>1.1000000000000001</v>
+        <v>7.1</v>
       </c>
       <c r="F29">
-        <v>10949</v>
+        <v>31601</v>
       </c>
       <c r="G29">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H29">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I29">
-        <v>56</v>
+        <v>37607</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B30" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="C30" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="D30">
-        <v>959</v>
+        <v>3931</v>
       </c>
       <c r="E30">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="F30">
-        <v>11546</v>
+        <v>26678</v>
       </c>
       <c r="G30">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H30">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="I30">
-        <v>31</v>
+        <v>47765</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B31" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="C31" t="s">
-        <v>53</v>
+        <v>38</v>
       </c>
       <c r="D31">
-        <v>1716</v>
+        <v>3931</v>
       </c>
       <c r="E31">
-        <v>1.4</v>
+        <v>6</v>
       </c>
       <c r="F31">
-        <v>11721</v>
+        <v>26542</v>
       </c>
       <c r="G31">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="H31">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="I31">
-        <v>52</v>
+        <v>46553</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B32" t="s">
-        <v>53</v>
+        <v>38</v>
       </c>
       <c r="C32" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="D32">
-        <v>528</v>
+        <v>4759</v>
       </c>
       <c r="E32">
-        <v>0.8</v>
+        <v>7.1</v>
       </c>
       <c r="F32">
-        <v>6601</v>
+        <v>31912</v>
       </c>
       <c r="G32">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="H32">
         <v>4</v>
       </c>
       <c r="I32">
-        <v>67</v>
+        <v>40982</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B33" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="C33" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="D33">
-        <v>1678</v>
+        <v>4759</v>
       </c>
       <c r="E33">
-        <v>1.4</v>
+        <v>7.1</v>
       </c>
       <c r="F33">
-        <v>11520</v>
+        <v>31601</v>
       </c>
       <c r="G33">
         <v>4</v>
       </c>
       <c r="H33">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I33">
-        <v>51</v>
+        <v>37607</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>12</v>
+      </c>
+      <c r="B34" t="s">
+        <v>38</v>
+      </c>
+      <c r="C34" t="s">
+        <v>60</v>
+      </c>
+      <c r="D34">
+        <v>2400</v>
+      </c>
+      <c r="E34">
+        <v>3.8</v>
+      </c>
+      <c r="F34">
+        <v>17325</v>
+      </c>
+      <c r="G34">
+        <v>2</v>
+      </c>
+      <c r="H34">
+        <v>3</v>
+      </c>
+      <c r="I34">
+        <v>47148</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>12</v>
+      </c>
+      <c r="B35" t="s">
+        <v>60</v>
+      </c>
+      <c r="C35" t="s">
+        <v>61</v>
+      </c>
+      <c r="D35">
+        <v>2097</v>
+      </c>
+      <c r="E35">
+        <v>3.4</v>
+      </c>
+      <c r="F35">
+        <v>15401</v>
+      </c>
+      <c r="G35">
+        <v>3</v>
+      </c>
+      <c r="H35">
+        <v>2</v>
+      </c>
+      <c r="I35">
+        <v>48747</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>12</v>
+      </c>
+      <c r="B36" t="s">
+        <v>61</v>
+      </c>
+      <c r="C36" t="s">
+        <v>38</v>
+      </c>
+      <c r="D36">
+        <v>1186</v>
+      </c>
+      <c r="E36">
+        <v>2.1</v>
+      </c>
+      <c r="F36">
+        <v>9765</v>
+      </c>
+      <c r="G36">
+        <v>2</v>
+      </c>
+      <c r="H36">
+        <v>2</v>
+      </c>
+      <c r="I36">
+        <v>46386</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>12</v>
+      </c>
+      <c r="B37" t="s">
+        <v>38</v>
+      </c>
+      <c r="C37" t="s">
+        <v>55</v>
+      </c>
+      <c r="D37">
+        <v>1950</v>
+      </c>
+      <c r="E37">
+        <v>3.2</v>
+      </c>
+      <c r="F37">
+        <v>14562</v>
+      </c>
+      <c r="G37">
+        <v>2</v>
+      </c>
+      <c r="H37">
+        <v>2</v>
+      </c>
+      <c r="I37">
+        <v>47462</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>12</v>
+      </c>
+      <c r="B38" t="s">
+        <v>55</v>
+      </c>
+      <c r="C38" t="s">
+        <v>56</v>
+      </c>
+      <c r="D38">
+        <v>181</v>
+      </c>
+      <c r="E38">
+        <v>0.8</v>
+      </c>
+      <c r="F38">
+        <v>3666</v>
+      </c>
+      <c r="G38">
+        <v>2</v>
+      </c>
+      <c r="H38">
+        <v>4</v>
+      </c>
+      <c r="I38">
+        <v>43984</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>12</v>
+      </c>
+      <c r="B39" t="s">
+        <v>56</v>
+      </c>
+      <c r="C39" t="s">
+        <v>38</v>
+      </c>
+      <c r="D39">
+        <v>1809</v>
+      </c>
+      <c r="E39">
+        <v>3</v>
+      </c>
+      <c r="F39">
+        <v>13568</v>
+      </c>
+      <c r="G39">
+        <v>4</v>
+      </c>
+      <c r="H39">
+        <v>2</v>
+      </c>
+      <c r="I39">
+        <v>41907</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>12</v>
+      </c>
+      <c r="B40" t="s">
+        <v>38</v>
+      </c>
+      <c r="C40" t="s">
+        <v>57</v>
+      </c>
+      <c r="D40">
+        <v>796</v>
+      </c>
+      <c r="E40">
+        <v>1.6</v>
+      </c>
+      <c r="F40">
+        <v>7395</v>
+      </c>
+      <c r="G40">
+        <v>2</v>
+      </c>
+      <c r="H40">
+        <v>3</v>
+      </c>
+      <c r="I40">
+        <v>45199</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>12</v>
+      </c>
+      <c r="B41" t="s">
+        <v>57</v>
+      </c>
+      <c r="C41" t="s">
+        <v>58</v>
+      </c>
+      <c r="D41">
+        <v>880</v>
+      </c>
+      <c r="E41">
+        <v>1.7</v>
+      </c>
+      <c r="F41">
+        <v>7927</v>
+      </c>
+      <c r="G41">
+        <v>3</v>
+      </c>
+      <c r="H41">
+        <v>2</v>
+      </c>
+      <c r="I41">
+        <v>43359</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>12</v>
+      </c>
+      <c r="B42" t="s">
+        <v>58</v>
+      </c>
+      <c r="C42" t="s">
+        <v>59</v>
+      </c>
+      <c r="D42">
+        <v>200</v>
+      </c>
+      <c r="E42">
+        <v>0.8</v>
+      </c>
+      <c r="F42">
+        <v>3818</v>
+      </c>
+      <c r="G42">
+        <v>2</v>
+      </c>
+      <c r="H42">
+        <v>5</v>
+      </c>
+      <c r="I42">
+        <v>41287</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>12</v>
+      </c>
+      <c r="B43" t="s">
+        <v>59</v>
+      </c>
+      <c r="C43" t="s">
+        <v>38</v>
+      </c>
+      <c r="D43">
+        <v>1504</v>
+      </c>
+      <c r="E43">
+        <v>2.6</v>
+      </c>
+      <c r="F43">
+        <v>11708</v>
+      </c>
+      <c r="G43">
+        <v>5</v>
+      </c>
+      <c r="H43">
+        <v>2</v>
+      </c>
+      <c r="I43">
+        <v>41972</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>12</v>
+      </c>
+      <c r="B44" t="s">
+        <v>38</v>
+      </c>
+      <c r="C44" t="s">
+        <v>57</v>
+      </c>
+      <c r="D44">
+        <v>796</v>
+      </c>
+      <c r="E44">
+        <v>1.6</v>
+      </c>
+      <c r="F44">
+        <v>7395</v>
+      </c>
+      <c r="G44">
+        <v>2</v>
+      </c>
+      <c r="H44">
+        <v>3</v>
+      </c>
+      <c r="I44">
+        <v>45199</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>12</v>
+      </c>
+      <c r="B45" t="s">
+        <v>57</v>
+      </c>
+      <c r="C45" t="s">
+        <v>58</v>
+      </c>
+      <c r="D45">
+        <v>880</v>
+      </c>
+      <c r="E45">
+        <v>1.7</v>
+      </c>
+      <c r="F45">
+        <v>7927</v>
+      </c>
+      <c r="G45">
+        <v>3</v>
+      </c>
+      <c r="H45">
+        <v>3</v>
+      </c>
+      <c r="I45">
+        <v>43359</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>12</v>
+      </c>
+      <c r="B46" t="s">
+        <v>58</v>
+      </c>
+      <c r="C46" t="s">
+        <v>59</v>
+      </c>
+      <c r="D46">
+        <v>200</v>
+      </c>
+      <c r="E46">
+        <v>0.8</v>
+      </c>
+      <c r="F46">
+        <v>3818</v>
+      </c>
+      <c r="G46">
+        <v>3</v>
+      </c>
+      <c r="H46">
+        <v>5</v>
+      </c>
+      <c r="I46">
+        <v>41287</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>12</v>
+      </c>
+      <c r="B47" t="s">
+        <v>59</v>
+      </c>
+      <c r="C47" t="s">
+        <v>38</v>
+      </c>
+      <c r="D47">
+        <v>1504</v>
+      </c>
+      <c r="E47">
+        <v>2.6</v>
+      </c>
+      <c r="F47">
+        <v>11708</v>
+      </c>
+      <c r="G47">
+        <v>5</v>
+      </c>
+      <c r="H47">
+        <v>2</v>
+      </c>
+      <c r="I47">
+        <v>41972</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>10</v>
+      </c>
+      <c r="B48" t="s">
+        <v>41</v>
+      </c>
+      <c r="C48" t="s">
+        <v>62</v>
+      </c>
+      <c r="D48">
+        <v>2876</v>
+      </c>
+      <c r="E48">
+        <v>7.4</v>
+      </c>
+      <c r="F48">
+        <v>12280</v>
+      </c>
+      <c r="G48">
+        <v>5</v>
+      </c>
+      <c r="H48">
+        <v>5</v>
+      </c>
+      <c r="I48">
+        <v>91473</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>10</v>
+      </c>
+      <c r="B49" t="s">
+        <v>62</v>
+      </c>
+      <c r="C49" t="s">
+        <v>37</v>
+      </c>
+      <c r="D49">
+        <v>2932</v>
+      </c>
+      <c r="E49">
+        <v>7.6</v>
+      </c>
+      <c r="F49">
+        <v>11845</v>
+      </c>
+      <c r="G49">
+        <v>5</v>
+      </c>
+      <c r="H49">
+        <v>5</v>
+      </c>
+      <c r="I49">
+        <v>64040</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>10</v>
+      </c>
+      <c r="B50" t="s">
+        <v>37</v>
+      </c>
+      <c r="C50" t="s">
+        <v>63</v>
+      </c>
+      <c r="D50">
+        <v>573</v>
+      </c>
+      <c r="E50">
+        <v>1.9</v>
+      </c>
+      <c r="F50">
+        <v>3164</v>
+      </c>
+      <c r="G50">
+        <v>5</v>
+      </c>
+      <c r="H50">
+        <v>5</v>
+      </c>
+      <c r="I50">
+        <v>20465</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>10</v>
+      </c>
+      <c r="B51" t="s">
+        <v>63</v>
+      </c>
+      <c r="C51" t="s">
+        <v>64</v>
+      </c>
+      <c r="D51">
+        <v>73</v>
+      </c>
+      <c r="E51">
+        <v>0.7</v>
+      </c>
+      <c r="F51">
+        <v>1242</v>
+      </c>
+      <c r="G51">
+        <v>5</v>
+      </c>
+      <c r="H51">
+        <v>5</v>
+      </c>
+      <c r="I51">
+        <v>95123</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>10</v>
+      </c>
+      <c r="B52" t="s">
+        <v>64</v>
+      </c>
+      <c r="C52" t="s">
+        <v>29</v>
+      </c>
+      <c r="D52">
+        <v>926</v>
+      </c>
+      <c r="E52">
+        <v>2.7</v>
+      </c>
+      <c r="F52">
+        <v>4440</v>
+      </c>
+      <c r="G52">
+        <v>5</v>
+      </c>
+      <c r="H52">
+        <v>5</v>
+      </c>
+      <c r="I52">
+        <v>91473</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>10</v>
+      </c>
+      <c r="B53" t="s">
+        <v>29</v>
+      </c>
+      <c r="C53" t="s">
+        <v>41</v>
+      </c>
+      <c r="D53">
+        <v>1604</v>
+      </c>
+      <c r="E53">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="F53">
+        <v>7367</v>
+      </c>
+      <c r="G53">
+        <v>5</v>
+      </c>
+      <c r="H53">
+        <v>5</v>
+      </c>
+      <c r="I53">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I47">
+    <sortCondition ref="A2:A47"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated planes.xlsx and refined work_order_generator.py logic
</commit_message>
<xml_diff>
--- a/planes.xlsx
+++ b/planes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aaron\OnAir\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFE2E665-1D86-465F-86B8-72D618E9A4D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8783EE2A-A1F9-44DD-ACA6-266E5AA4DBDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30630" yWindow="3390" windowWidth="21600" windowHeight="12645" activeTab="1" xr2:uid="{7DA1CCB9-1292-47D3-ABC3-3EB19435A409}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{7DA1CCB9-1292-47D3-ABC3-3EB19435A409}"/>
   </bookViews>
   <sheets>
     <sheet name="Planes" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="99">
   <si>
     <t>Plane</t>
   </si>
@@ -229,13 +229,115 @@
   </si>
   <si>
     <t>KCVG</t>
+  </si>
+  <si>
+    <t>KSEA</t>
+  </si>
+  <si>
+    <t>ESGG</t>
+  </si>
+  <si>
+    <t>KORD</t>
+  </si>
+  <si>
+    <t>MDLR</t>
+  </si>
+  <si>
+    <t>KCEF</t>
+  </si>
+  <si>
+    <t>KDHN</t>
+  </si>
+  <si>
+    <t>KMGE</t>
+  </si>
+  <si>
+    <t>KBNA</t>
+  </si>
+  <si>
+    <t>KDAY</t>
+  </si>
+  <si>
+    <t>KHSV</t>
+  </si>
+  <si>
+    <t>KMIA</t>
+  </si>
+  <si>
+    <t>KJAX</t>
+  </si>
+  <si>
+    <t>Cessna Longitude</t>
+  </si>
+  <si>
+    <t>KADW</t>
+  </si>
+  <si>
+    <t>EINN</t>
+  </si>
+  <si>
+    <t>Vertigo - Turbo Prop Racer</t>
+  </si>
+  <si>
+    <t>KMRB</t>
+  </si>
+  <si>
+    <t>KMEM</t>
+  </si>
+  <si>
+    <t>CYOD</t>
+  </si>
+  <si>
+    <t>KDAL</t>
+  </si>
+  <si>
+    <t>KMTJ</t>
+  </si>
+  <si>
+    <t>KDSM</t>
+  </si>
+  <si>
+    <t>KBTL</t>
+  </si>
+  <si>
+    <t>KIND</t>
+  </si>
+  <si>
+    <t>KNFW</t>
+  </si>
+  <si>
+    <t>KEFD</t>
+  </si>
+  <si>
+    <t>KXNA</t>
+  </si>
+  <si>
+    <t>KTOL</t>
+  </si>
+  <si>
+    <t>KCLE</t>
+  </si>
+  <si>
+    <t>KEWR</t>
+  </si>
+  <si>
+    <t>KBOS</t>
+  </si>
+  <si>
+    <t>KBTV</t>
+  </si>
+  <si>
+    <t>KROC</t>
+  </si>
+  <si>
+    <t>TFFR</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -366,6 +468,12 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1089,10 +1197,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A16643A-B77F-44B3-83CF-168AF5426912}">
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1261,16 +1369,16 @@
         <v>0</v>
       </c>
       <c r="D6">
-        <v>1901</v>
+        <v>1806</v>
       </c>
       <c r="E6">
-        <v>10036</v>
+        <v>9390</v>
       </c>
       <c r="F6">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="G6">
-        <v>14502</v>
+        <v>13620</v>
       </c>
       <c r="H6" t="s">
         <v>15</v>
@@ -1335,6 +1443,35 @@
       </c>
       <c r="I8" t="s">
         <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>80</v>
+      </c>
+      <c r="B9">
+        <v>320</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>1044</v>
+      </c>
+      <c r="E9">
+        <v>219</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <v>800</v>
+      </c>
+      <c r="H9" t="s">
+        <v>9</v>
+      </c>
+      <c r="I9" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -1344,16 +1481,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B22E5411-C937-41B5-8075-5A67875F9274}">
-  <dimension ref="A1:I53"/>
+  <dimension ref="A1:I108"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A52" sqref="A52"/>
+      <pane ySplit="1" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A108" sqref="A108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.7109375" bestFit="1" customWidth="1"/>
@@ -1655,80 +1792,80 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>41</v>
+        <v>82</v>
       </c>
       <c r="C11" t="s">
-        <v>42</v>
+        <v>83</v>
       </c>
       <c r="D11">
-        <v>1983</v>
+        <v>1438</v>
       </c>
       <c r="E11">
-        <v>2.2000000000000002</v>
+        <v>3.1</v>
       </c>
       <c r="F11">
-        <v>21251</v>
+        <v>20030</v>
       </c>
       <c r="G11">
         <v>5</v>
       </c>
       <c r="H11">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I11">
-        <v>12106</v>
+        <v>547507</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B12" t="s">
-        <v>42</v>
+        <v>83</v>
       </c>
       <c r="C12" t="s">
-        <v>43</v>
+        <v>84</v>
       </c>
       <c r="D12">
-        <v>1548</v>
+        <v>1413</v>
       </c>
       <c r="E12">
-        <v>1.8</v>
+        <v>3.1</v>
       </c>
       <c r="F12">
-        <v>17679</v>
+        <v>18887</v>
       </c>
       <c r="G12">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H12">
         <v>4</v>
       </c>
       <c r="I12">
-        <v>3318</v>
+        <v>651579</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B13" t="s">
-        <v>43</v>
+        <v>84</v>
       </c>
       <c r="C13" t="s">
-        <v>44</v>
+        <v>85</v>
       </c>
       <c r="D13">
-        <v>415</v>
+        <v>636</v>
       </c>
       <c r="E13">
-        <v>0.9</v>
+        <v>1.7</v>
       </c>
       <c r="F13">
-        <v>8443</v>
+        <v>10576</v>
       </c>
       <c r="G13">
         <v>4</v>
@@ -1737,172 +1874,172 @@
         <v>4</v>
       </c>
       <c r="I13">
-        <v>25201</v>
+        <v>635988</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B14" t="s">
-        <v>44</v>
+        <v>85</v>
       </c>
       <c r="C14" t="s">
-        <v>45</v>
+        <v>82</v>
       </c>
       <c r="D14">
-        <v>1954</v>
+        <v>884</v>
       </c>
       <c r="E14">
-        <v>2.2000000000000002</v>
+        <v>2.1</v>
       </c>
       <c r="F14">
-        <v>20857</v>
+        <v>13726</v>
       </c>
       <c r="G14">
         <v>4</v>
       </c>
       <c r="H14">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I14">
-        <v>22586</v>
+        <v>524914</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B15" t="s">
-        <v>45</v>
+        <v>82</v>
       </c>
       <c r="C15" t="s">
-        <v>41</v>
+        <v>86</v>
       </c>
       <c r="D15">
-        <v>3037</v>
+        <v>426</v>
       </c>
       <c r="E15">
-        <v>3.1</v>
+        <v>1.3</v>
       </c>
       <c r="F15">
-        <v>30551</v>
+        <v>8511</v>
       </c>
       <c r="G15">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H15">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I15">
-        <v>19837</v>
+        <v>591735</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B16" t="s">
-        <v>41</v>
+        <v>86</v>
       </c>
       <c r="C16" t="s">
-        <v>46</v>
+        <v>87</v>
       </c>
       <c r="D16">
-        <v>2727</v>
+        <v>378</v>
       </c>
       <c r="E16">
-        <v>2.8</v>
+        <v>1.2</v>
       </c>
       <c r="F16">
-        <v>27806</v>
+        <v>7482</v>
       </c>
       <c r="G16">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H16">
         <v>4</v>
       </c>
       <c r="I16">
-        <v>9758</v>
+        <v>524942</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B17" t="s">
-        <v>46</v>
+        <v>87</v>
       </c>
       <c r="C17" t="s">
-        <v>47</v>
+        <v>88</v>
       </c>
       <c r="D17">
-        <v>2034</v>
+        <v>162</v>
       </c>
       <c r="E17">
-        <v>2.2000000000000002</v>
+        <v>0.8</v>
       </c>
       <c r="F17">
-        <v>24970</v>
+        <v>5281</v>
       </c>
       <c r="G17">
         <v>4</v>
       </c>
       <c r="H17">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I17">
-        <v>14131</v>
+        <v>659652</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B18" t="s">
-        <v>47</v>
+        <v>88</v>
       </c>
       <c r="C18" t="s">
-        <v>48</v>
+        <v>82</v>
       </c>
       <c r="D18">
-        <v>1100</v>
+        <v>331</v>
       </c>
       <c r="E18">
-        <v>1.4</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="F18">
-        <v>14081</v>
+        <v>7722</v>
       </c>
       <c r="G18">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H18">
         <v>5</v>
       </c>
       <c r="I18">
-        <v>27903</v>
+        <v>563761</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B19" t="s">
-        <v>48</v>
+        <v>82</v>
       </c>
       <c r="C19" t="s">
-        <v>41</v>
+        <v>89</v>
       </c>
       <c r="D19">
-        <v>226</v>
+        <v>396</v>
       </c>
       <c r="E19">
-        <v>0.7</v>
+        <v>1.2</v>
       </c>
       <c r="F19">
-        <v>7917</v>
+        <v>7944</v>
       </c>
       <c r="G19">
         <v>5</v>
@@ -1911,926 +2048,926 @@
         <v>5</v>
       </c>
       <c r="I19">
-        <v>31131</v>
+        <v>502109</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="B20" t="s">
-        <v>49</v>
+        <v>89</v>
       </c>
       <c r="C20" t="s">
-        <v>50</v>
+        <v>90</v>
       </c>
       <c r="D20">
-        <v>306</v>
+        <v>223</v>
       </c>
       <c r="E20">
-        <v>0.7</v>
+        <v>0.9</v>
       </c>
       <c r="F20">
-        <v>6179</v>
+        <v>6515</v>
       </c>
       <c r="G20">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="H20">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I20">
-        <v>61</v>
+        <v>649527</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="B21" t="s">
-        <v>50</v>
+        <v>90</v>
       </c>
       <c r="C21" t="s">
-        <v>51</v>
+        <v>82</v>
       </c>
       <c r="D21">
-        <v>1084</v>
+        <v>419</v>
       </c>
       <c r="E21">
-        <v>1.1000000000000001</v>
+        <v>1.3</v>
       </c>
       <c r="F21">
-        <v>10949</v>
+        <v>8675</v>
       </c>
       <c r="G21">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H21">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I21">
-        <v>56</v>
+        <v>534672</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="B22" t="s">
-        <v>51</v>
+        <v>82</v>
       </c>
       <c r="C22" t="s">
-        <v>52</v>
+        <v>91</v>
       </c>
       <c r="D22">
-        <v>959</v>
+        <v>224</v>
       </c>
       <c r="E22">
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="F22">
-        <v>11546</v>
+        <v>6027</v>
       </c>
       <c r="G22">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H22">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I22">
-        <v>31</v>
+        <v>526393</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="B23" t="s">
-        <v>49</v>
+        <v>91</v>
       </c>
       <c r="C23" t="s">
-        <v>53</v>
+        <v>82</v>
       </c>
       <c r="D23">
-        <v>1716</v>
+        <v>224</v>
       </c>
       <c r="E23">
-        <v>1.4</v>
+        <v>0.9</v>
       </c>
       <c r="F23">
-        <v>11721</v>
+        <v>6562</v>
       </c>
       <c r="G23">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H23">
         <v>5</v>
       </c>
       <c r="I23">
-        <v>52</v>
+        <v>511605</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="B24" t="s">
-        <v>53</v>
+        <v>82</v>
       </c>
       <c r="C24" t="s">
-        <v>54</v>
+        <v>92</v>
       </c>
       <c r="D24">
-        <v>528</v>
+        <v>488</v>
       </c>
       <c r="E24">
-        <v>0.8</v>
+        <v>1.4</v>
       </c>
       <c r="F24">
-        <v>6601</v>
+        <v>8886</v>
       </c>
       <c r="G24">
         <v>5</v>
       </c>
       <c r="H24">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I24">
-        <v>67</v>
+        <v>612508</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="B25" t="s">
-        <v>54</v>
+        <v>92</v>
       </c>
       <c r="C25" t="s">
-        <v>49</v>
+        <v>93</v>
       </c>
       <c r="D25">
-        <v>1678</v>
+        <v>88</v>
       </c>
       <c r="E25">
-        <v>1.4</v>
+        <v>0.7</v>
       </c>
       <c r="F25">
-        <v>11520</v>
+        <v>4524</v>
       </c>
       <c r="G25">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H25">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I25">
-        <v>51</v>
+        <v>639327</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B26" t="s">
-        <v>38</v>
+        <v>93</v>
       </c>
       <c r="C26" t="s">
-        <v>39</v>
+        <v>82</v>
       </c>
       <c r="D26">
-        <v>3931</v>
+        <v>540</v>
       </c>
       <c r="E26">
-        <v>6</v>
+        <v>1.5</v>
       </c>
       <c r="F26">
-        <v>26678</v>
+        <v>9995</v>
       </c>
       <c r="G26">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H26">
         <v>5</v>
       </c>
       <c r="I26">
-        <v>47765</v>
+        <v>609743</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B27" t="s">
-        <v>39</v>
+        <v>82</v>
       </c>
       <c r="C27" t="s">
-        <v>38</v>
+        <v>94</v>
       </c>
       <c r="D27">
-        <v>3931</v>
+        <v>820</v>
       </c>
       <c r="E27">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F27">
-        <v>26542</v>
+        <v>12077</v>
       </c>
       <c r="G27">
         <v>5</v>
       </c>
       <c r="H27">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="I27">
-        <v>46553</v>
+        <v>581601</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B28" t="s">
-        <v>38</v>
+        <v>94</v>
       </c>
       <c r="C28" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D28">
-        <v>4759</v>
+        <v>341</v>
       </c>
       <c r="E28">
-        <v>7.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="F28">
-        <v>31912</v>
+        <v>8574</v>
       </c>
       <c r="G28">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H28">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I28">
-        <v>40982</v>
+        <v>543599</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B29" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C29" t="s">
-        <v>38</v>
+        <v>79</v>
       </c>
       <c r="D29">
-        <v>4759</v>
+        <v>2345</v>
       </c>
       <c r="E29">
-        <v>7.1</v>
+        <v>4.8</v>
       </c>
       <c r="F29">
-        <v>31601</v>
+        <v>29561</v>
       </c>
       <c r="G29">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H29">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="I29">
-        <v>37607</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B30" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C30" t="s">
-        <v>39</v>
+        <v>62</v>
       </c>
       <c r="D30">
-        <v>3931</v>
+        <v>2876</v>
       </c>
       <c r="E30">
-        <v>6</v>
+        <v>5.7</v>
       </c>
       <c r="F30">
-        <v>26678</v>
+        <v>36636</v>
       </c>
       <c r="G30">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H30">
         <v>5</v>
       </c>
       <c r="I30">
-        <v>47765</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B31" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C31" t="s">
-        <v>38</v>
+        <v>95</v>
       </c>
       <c r="D31">
-        <v>3931</v>
+        <v>175</v>
       </c>
       <c r="E31">
-        <v>6</v>
+        <v>0.8</v>
       </c>
       <c r="F31">
-        <v>26542</v>
+        <v>5300</v>
       </c>
       <c r="G31">
         <v>5</v>
       </c>
       <c r="H31">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="I31">
-        <v>46553</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B32" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C32" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D32">
-        <v>4759</v>
+        <v>332</v>
       </c>
       <c r="E32">
-        <v>7.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="F32">
-        <v>31912</v>
+        <v>7154</v>
       </c>
       <c r="G32">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H32">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I32">
-        <v>40982</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B33" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C33" t="s">
-        <v>38</v>
+        <v>75</v>
       </c>
       <c r="D33">
-        <v>4759</v>
+        <v>1268</v>
       </c>
       <c r="E33">
-        <v>7.1</v>
+        <v>2.8</v>
       </c>
       <c r="F33">
-        <v>31601</v>
+        <v>17330</v>
       </c>
       <c r="G33">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H33">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="I33">
-        <v>37607</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B34" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C34" t="s">
-        <v>60</v>
+        <v>78</v>
       </c>
       <c r="D34">
-        <v>2400</v>
+        <v>508</v>
       </c>
       <c r="E34">
-        <v>3.8</v>
+        <v>1.4</v>
       </c>
       <c r="F34">
-        <v>17325</v>
+        <v>8753</v>
       </c>
       <c r="G34">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H34">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="I34">
-        <v>47148</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B35" t="s">
-        <v>60</v>
+        <v>41</v>
       </c>
       <c r="C35" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D35">
-        <v>2097</v>
+        <v>2876</v>
       </c>
       <c r="E35">
-        <v>3.4</v>
+        <v>7.4</v>
       </c>
       <c r="F35">
-        <v>15401</v>
+        <v>12280</v>
       </c>
       <c r="G35">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H35">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="I35">
-        <v>48747</v>
+        <v>91473</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B36" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C36" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D36">
-        <v>1186</v>
+        <v>2932</v>
       </c>
       <c r="E36">
-        <v>2.1</v>
+        <v>7.6</v>
       </c>
       <c r="F36">
-        <v>9765</v>
+        <v>11845</v>
       </c>
       <c r="G36">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H36">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="I36">
-        <v>46386</v>
+        <v>64040</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B37" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C37" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="D37">
-        <v>1950</v>
+        <v>573</v>
       </c>
       <c r="E37">
-        <v>3.2</v>
+        <v>1.9</v>
       </c>
       <c r="F37">
-        <v>14562</v>
+        <v>3164</v>
       </c>
       <c r="G37">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H37">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="I37">
-        <v>47462</v>
+        <v>20465</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B38" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="C38" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="D38">
-        <v>181</v>
+        <v>73</v>
       </c>
       <c r="E38">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="F38">
-        <v>3666</v>
+        <v>1242</v>
       </c>
       <c r="G38">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H38">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I38">
-        <v>43984</v>
+        <v>95123</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B39" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="C39" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="D39">
-        <v>1809</v>
+        <v>926</v>
       </c>
       <c r="E39">
-        <v>3</v>
+        <v>2.7</v>
       </c>
       <c r="F39">
-        <v>13568</v>
+        <v>4440</v>
       </c>
       <c r="G39">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H39">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="I39">
-        <v>41907</v>
+        <v>91473</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B40" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="C40" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="D40">
-        <v>796</v>
+        <v>1604</v>
       </c>
       <c r="E40">
-        <v>1.6</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="F40">
-        <v>7395</v>
+        <v>7367</v>
       </c>
       <c r="G40">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H40">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="I40">
-        <v>45199</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>12</v>
+        <v>77</v>
       </c>
       <c r="B41" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="C41" t="s">
-        <v>58</v>
+        <v>78</v>
       </c>
       <c r="D41">
-        <v>880</v>
+        <v>508</v>
       </c>
       <c r="E41">
-        <v>1.7</v>
+        <v>1.6</v>
       </c>
       <c r="F41">
-        <v>7927</v>
+        <v>477</v>
       </c>
       <c r="G41">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H41">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="I41">
-        <v>43359</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>12</v>
+        <v>77</v>
       </c>
       <c r="B42" t="s">
-        <v>58</v>
+        <v>78</v>
       </c>
       <c r="C42" t="s">
-        <v>59</v>
+        <v>79</v>
       </c>
       <c r="D42">
-        <v>200</v>
+        <v>2849</v>
       </c>
       <c r="E42">
-        <v>0.8</v>
+        <v>6.4</v>
       </c>
       <c r="F42">
-        <v>3818</v>
+        <v>1972</v>
       </c>
       <c r="G42">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H42">
         <v>5</v>
       </c>
       <c r="I42">
-        <v>41287</v>
+        <v>1863</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B43" t="s">
-        <v>59</v>
+        <v>41</v>
       </c>
       <c r="C43" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="D43">
-        <v>1504</v>
+        <v>1983</v>
       </c>
       <c r="E43">
-        <v>2.6</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="F43">
-        <v>11708</v>
+        <v>21251</v>
       </c>
       <c r="G43">
         <v>5</v>
       </c>
       <c r="H43">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I43">
-        <v>41972</v>
+        <v>12106</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B44" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C44" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D44">
-        <v>796</v>
+        <v>1548</v>
       </c>
       <c r="E44">
-        <v>1.6</v>
+        <v>1.8</v>
       </c>
       <c r="F44">
-        <v>7395</v>
+        <v>17679</v>
       </c>
       <c r="G44">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H44">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I44">
-        <v>45199</v>
+        <v>3318</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B45" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="C45" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="D45">
-        <v>880</v>
+        <v>415</v>
       </c>
       <c r="E45">
-        <v>1.7</v>
+        <v>0.9</v>
       </c>
       <c r="F45">
-        <v>7927</v>
+        <v>8443</v>
       </c>
       <c r="G45">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H45">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I45">
-        <v>43359</v>
+        <v>25201</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B46" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="C46" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="D46">
-        <v>200</v>
+        <v>1954</v>
       </c>
       <c r="E46">
-        <v>0.8</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="F46">
-        <v>3818</v>
+        <v>20857</v>
       </c>
       <c r="G46">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H46">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I46">
-        <v>41287</v>
+        <v>22586</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B47" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="C47" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="D47">
-        <v>1504</v>
+        <v>3037</v>
       </c>
       <c r="E47">
-        <v>2.6</v>
+        <v>3.1</v>
       </c>
       <c r="F47">
-        <v>11708</v>
+        <v>30551</v>
       </c>
       <c r="G47">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H47">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="I47">
-        <v>41972</v>
+        <v>19837</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B48" t="s">
         <v>41</v>
       </c>
       <c r="C48" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="D48">
-        <v>2876</v>
+        <v>2727</v>
       </c>
       <c r="E48">
-        <v>7.4</v>
+        <v>2.8</v>
       </c>
       <c r="F48">
-        <v>12280</v>
+        <v>27806</v>
       </c>
       <c r="G48">
         <v>5</v>
       </c>
       <c r="H48">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I48">
-        <v>91473</v>
+        <v>9758</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B49" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="C49" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="D49">
-        <v>2932</v>
+        <v>2034</v>
       </c>
       <c r="E49">
-        <v>7.6</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="F49">
-        <v>11845</v>
+        <v>24970</v>
       </c>
       <c r="G49">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H49">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I49">
-        <v>64040</v>
+        <v>14131</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B50" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="C50" t="s">
-        <v>63</v>
+        <v>48</v>
       </c>
       <c r="D50">
-        <v>573</v>
+        <v>1100</v>
       </c>
       <c r="E50">
-        <v>1.9</v>
+        <v>1.4</v>
       </c>
       <c r="F50">
-        <v>3164</v>
+        <v>14081</v>
       </c>
       <c r="G50">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H50">
         <v>5</v>
       </c>
       <c r="I50">
-        <v>20465</v>
+        <v>27903</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B51" t="s">
-        <v>63</v>
+        <v>48</v>
       </c>
       <c r="C51" t="s">
-        <v>64</v>
+        <v>41</v>
       </c>
       <c r="D51">
-        <v>73</v>
+        <v>226</v>
       </c>
       <c r="E51">
         <v>0.7</v>
       </c>
       <c r="F51">
-        <v>1242</v>
+        <v>7917</v>
       </c>
       <c r="G51">
         <v>5</v>
@@ -2839,71 +2976,1667 @@
         <v>5</v>
       </c>
       <c r="I51">
-        <v>95123</v>
+        <v>31131</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B52" t="s">
-        <v>64</v>
+        <v>41</v>
       </c>
       <c r="C52" t="s">
-        <v>29</v>
+        <v>68</v>
       </c>
       <c r="D52">
-        <v>926</v>
+        <v>1581</v>
       </c>
       <c r="E52">
-        <v>2.7</v>
+        <v>1.9</v>
       </c>
       <c r="F52">
-        <v>4440</v>
+        <v>18239</v>
       </c>
       <c r="G52">
         <v>5</v>
       </c>
       <c r="H52">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I52">
-        <v>91473</v>
+        <v>562</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B53" t="s">
-        <v>29</v>
+        <v>68</v>
       </c>
       <c r="C53" t="s">
         <v>41</v>
       </c>
       <c r="D53">
-        <v>1604</v>
+        <v>1581</v>
       </c>
       <c r="E53">
-        <v>4.4000000000000004</v>
+        <v>1.9</v>
       </c>
       <c r="F53">
-        <v>7367</v>
+        <v>18827</v>
       </c>
       <c r="G53">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H53">
         <v>5</v>
       </c>
       <c r="I53">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>13</v>
+      </c>
+      <c r="B54" t="s">
+        <v>41</v>
+      </c>
+      <c r="C54" t="s">
+        <v>69</v>
+      </c>
+      <c r="D54">
+        <v>225</v>
+      </c>
+      <c r="E54">
+        <v>0.7</v>
+      </c>
+      <c r="F54">
+        <v>6997</v>
+      </c>
+      <c r="G54">
+        <v>5</v>
+      </c>
+      <c r="H54">
+        <v>5</v>
+      </c>
+      <c r="I54">
+        <v>29652</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>13</v>
+      </c>
+      <c r="B55" t="s">
+        <v>69</v>
+      </c>
+      <c r="C55" t="s">
+        <v>70</v>
+      </c>
+      <c r="D55">
+        <v>899</v>
+      </c>
+      <c r="E55">
+        <v>1.3</v>
+      </c>
+      <c r="F55">
+        <v>12440</v>
+      </c>
+      <c r="G55">
+        <v>5</v>
+      </c>
+      <c r="H55">
+        <v>4</v>
+      </c>
+      <c r="I55">
+        <v>2732</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>13</v>
+      </c>
+      <c r="B56" t="s">
+        <v>70</v>
+      </c>
+      <c r="C56" t="s">
+        <v>41</v>
+      </c>
+      <c r="D56">
+        <v>1123</v>
+      </c>
+      <c r="E56">
+        <v>1.5</v>
+      </c>
+      <c r="F56">
+        <v>15139</v>
+      </c>
+      <c r="G56">
+        <v>4</v>
+      </c>
+      <c r="H56">
+        <v>5</v>
+      </c>
+      <c r="I56">
+        <v>28914</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>13</v>
+      </c>
+      <c r="B57" t="s">
+        <v>41</v>
+      </c>
+      <c r="C57" t="s">
+        <v>71</v>
+      </c>
+      <c r="D57">
+        <v>975</v>
+      </c>
+      <c r="E57">
+        <v>1.3</v>
+      </c>
+      <c r="F57">
+        <v>13014</v>
+      </c>
+      <c r="G57">
+        <v>5</v>
+      </c>
+      <c r="H57">
+        <v>4</v>
+      </c>
+      <c r="I57">
+        <v>9194</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>13</v>
+      </c>
+      <c r="B58" t="s">
+        <v>71</v>
+      </c>
+      <c r="C58" t="s">
+        <v>72</v>
+      </c>
+      <c r="D58">
+        <v>170</v>
+      </c>
+      <c r="E58">
+        <v>0.6</v>
+      </c>
+      <c r="F58">
+        <v>6142</v>
+      </c>
+      <c r="G58">
+        <v>4</v>
+      </c>
+      <c r="H58">
+        <v>5</v>
+      </c>
+      <c r="I58">
+        <v>12540</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>13</v>
+      </c>
+      <c r="B59" t="s">
+        <v>72</v>
+      </c>
+      <c r="C59" t="s">
+        <v>41</v>
+      </c>
+      <c r="D59">
+        <v>964</v>
+      </c>
+      <c r="E59">
+        <v>1.3</v>
+      </c>
+      <c r="F59">
+        <v>13856</v>
+      </c>
+      <c r="G59">
+        <v>5</v>
+      </c>
+      <c r="H59">
+        <v>5</v>
+      </c>
+      <c r="I59">
+        <v>2367</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>13</v>
+      </c>
+      <c r="B60" t="s">
+        <v>41</v>
+      </c>
+      <c r="C60" t="s">
+        <v>73</v>
+      </c>
+      <c r="D60">
+        <v>742</v>
+      </c>
+      <c r="E60">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F60">
+        <v>11106</v>
+      </c>
+      <c r="G60">
+        <v>5</v>
+      </c>
+      <c r="H60">
+        <v>5</v>
+      </c>
+      <c r="I60">
+        <v>8355</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>13</v>
+      </c>
+      <c r="B61" t="s">
+        <v>73</v>
+      </c>
+      <c r="C61" t="s">
+        <v>74</v>
+      </c>
+      <c r="D61">
+        <v>339</v>
+      </c>
+      <c r="E61">
+        <v>0.8</v>
+      </c>
+      <c r="F61">
+        <v>7935</v>
+      </c>
+      <c r="G61">
+        <v>5</v>
+      </c>
+      <c r="H61">
+        <v>5</v>
+      </c>
+      <c r="I61">
+        <v>23387</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>13</v>
+      </c>
+      <c r="B62" t="s">
+        <v>74</v>
+      </c>
+      <c r="C62" t="s">
+        <v>41</v>
+      </c>
+      <c r="D62">
+        <v>1025</v>
+      </c>
+      <c r="E62">
+        <v>1.4</v>
+      </c>
+      <c r="F62">
+        <v>14348</v>
+      </c>
+      <c r="G62">
+        <v>5</v>
+      </c>
+      <c r="H62">
+        <v>5</v>
+      </c>
+      <c r="I62">
+        <v>12855</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>13</v>
+      </c>
+      <c r="B63" t="s">
+        <v>41</v>
+      </c>
+      <c r="C63" t="s">
+        <v>75</v>
+      </c>
+      <c r="D63">
+        <v>1268</v>
+      </c>
+      <c r="E63">
+        <v>1.6</v>
+      </c>
+      <c r="F63">
+        <v>15339</v>
+      </c>
+      <c r="G63">
+        <v>5</v>
+      </c>
+      <c r="H63">
+        <v>5</v>
+      </c>
+      <c r="I63">
         <v>0</v>
       </c>
     </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>13</v>
+      </c>
+      <c r="B64" t="s">
+        <v>75</v>
+      </c>
+      <c r="C64" t="s">
+        <v>65</v>
+      </c>
+      <c r="D64">
+        <v>2363</v>
+      </c>
+      <c r="E64">
+        <v>2.5</v>
+      </c>
+      <c r="F64">
+        <v>23877</v>
+      </c>
+      <c r="G64">
+        <v>5</v>
+      </c>
+      <c r="H64">
+        <v>5</v>
+      </c>
+      <c r="I64">
+        <v>13344</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>13</v>
+      </c>
+      <c r="B65" t="s">
+        <v>41</v>
+      </c>
+      <c r="C65" t="s">
+        <v>76</v>
+      </c>
+      <c r="D65">
+        <v>1051</v>
+      </c>
+      <c r="E65">
+        <v>1.4</v>
+      </c>
+      <c r="F65">
+        <v>13255</v>
+      </c>
+      <c r="G65">
+        <v>5</v>
+      </c>
+      <c r="H65">
+        <v>4</v>
+      </c>
+      <c r="I65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>17</v>
+      </c>
+      <c r="B66" t="s">
+        <v>41</v>
+      </c>
+      <c r="C66" t="s">
+        <v>38</v>
+      </c>
+      <c r="D66">
+        <v>51</v>
+      </c>
+      <c r="E66">
+        <v>0.8</v>
+      </c>
+      <c r="F66">
+        <v>415</v>
+      </c>
+      <c r="G66">
+        <v>5</v>
+      </c>
+      <c r="H66">
+        <v>2</v>
+      </c>
+      <c r="I66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>17</v>
+      </c>
+      <c r="B67" t="s">
+        <v>38</v>
+      </c>
+      <c r="C67" t="s">
+        <v>49</v>
+      </c>
+      <c r="D67">
+        <v>18</v>
+      </c>
+      <c r="E67">
+        <v>0.6</v>
+      </c>
+      <c r="F67">
+        <v>412</v>
+      </c>
+      <c r="G67">
+        <v>2</v>
+      </c>
+      <c r="H67">
+        <v>1</v>
+      </c>
+      <c r="I67">
+        <v>80278</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>17</v>
+      </c>
+      <c r="B68" t="s">
+        <v>49</v>
+      </c>
+      <c r="C68" t="s">
+        <v>41</v>
+      </c>
+      <c r="D68">
+        <v>36</v>
+      </c>
+      <c r="E68">
+        <v>0.7</v>
+      </c>
+      <c r="F68">
+        <v>669</v>
+      </c>
+      <c r="G68">
+        <v>1</v>
+      </c>
+      <c r="H68">
+        <v>5</v>
+      </c>
+      <c r="I68">
+        <v>7393</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>16</v>
+      </c>
+      <c r="B69" t="s">
+        <v>49</v>
+      </c>
+      <c r="C69" t="s">
+        <v>50</v>
+      </c>
+      <c r="D69">
+        <v>306</v>
+      </c>
+      <c r="E69">
+        <v>0.7</v>
+      </c>
+      <c r="F69">
+        <v>6179</v>
+      </c>
+      <c r="G69">
+        <v>1</v>
+      </c>
+      <c r="H69">
+        <v>3</v>
+      </c>
+      <c r="I69">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>16</v>
+      </c>
+      <c r="B70" t="s">
+        <v>50</v>
+      </c>
+      <c r="C70" t="s">
+        <v>51</v>
+      </c>
+      <c r="D70">
+        <v>1084</v>
+      </c>
+      <c r="E70">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F70">
+        <v>10949</v>
+      </c>
+      <c r="G70">
+        <v>3</v>
+      </c>
+      <c r="H70">
+        <v>4</v>
+      </c>
+      <c r="I70">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>16</v>
+      </c>
+      <c r="B71" t="s">
+        <v>51</v>
+      </c>
+      <c r="C71" t="s">
+        <v>52</v>
+      </c>
+      <c r="D71">
+        <v>959</v>
+      </c>
+      <c r="E71">
+        <v>1</v>
+      </c>
+      <c r="F71">
+        <v>11546</v>
+      </c>
+      <c r="G71">
+        <v>4</v>
+      </c>
+      <c r="H71">
+        <v>3</v>
+      </c>
+      <c r="I71">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>16</v>
+      </c>
+      <c r="B72" t="s">
+        <v>49</v>
+      </c>
+      <c r="C72" t="s">
+        <v>53</v>
+      </c>
+      <c r="D72">
+        <v>1716</v>
+      </c>
+      <c r="E72">
+        <v>1.4</v>
+      </c>
+      <c r="F72">
+        <v>11721</v>
+      </c>
+      <c r="G72">
+        <v>1</v>
+      </c>
+      <c r="H72">
+        <v>5</v>
+      </c>
+      <c r="I72">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>16</v>
+      </c>
+      <c r="B73" t="s">
+        <v>53</v>
+      </c>
+      <c r="C73" t="s">
+        <v>54</v>
+      </c>
+      <c r="D73">
+        <v>528</v>
+      </c>
+      <c r="E73">
+        <v>0.8</v>
+      </c>
+      <c r="F73">
+        <v>6601</v>
+      </c>
+      <c r="G73">
+        <v>5</v>
+      </c>
+      <c r="H73">
+        <v>4</v>
+      </c>
+      <c r="I73">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>16</v>
+      </c>
+      <c r="B74" t="s">
+        <v>54</v>
+      </c>
+      <c r="C74" t="s">
+        <v>49</v>
+      </c>
+      <c r="D74">
+        <v>1678</v>
+      </c>
+      <c r="E74">
+        <v>1.4</v>
+      </c>
+      <c r="F74">
+        <v>11520</v>
+      </c>
+      <c r="G74">
+        <v>4</v>
+      </c>
+      <c r="H74">
+        <v>1</v>
+      </c>
+      <c r="I74">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>12</v>
+      </c>
+      <c r="B75" t="s">
+        <v>38</v>
+      </c>
+      <c r="C75" t="s">
+        <v>39</v>
+      </c>
+      <c r="D75">
+        <v>3931</v>
+      </c>
+      <c r="E75">
+        <v>6</v>
+      </c>
+      <c r="F75">
+        <v>26678</v>
+      </c>
+      <c r="G75">
+        <v>2</v>
+      </c>
+      <c r="H75">
+        <v>5</v>
+      </c>
+      <c r="I75">
+        <v>47765</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>12</v>
+      </c>
+      <c r="B76" t="s">
+        <v>39</v>
+      </c>
+      <c r="C76" t="s">
+        <v>38</v>
+      </c>
+      <c r="D76">
+        <v>3931</v>
+      </c>
+      <c r="E76">
+        <v>6</v>
+      </c>
+      <c r="F76">
+        <v>26542</v>
+      </c>
+      <c r="G76">
+        <v>5</v>
+      </c>
+      <c r="H76">
+        <v>2</v>
+      </c>
+      <c r="I76">
+        <v>46553</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>12</v>
+      </c>
+      <c r="B77" t="s">
+        <v>38</v>
+      </c>
+      <c r="C77" t="s">
+        <v>40</v>
+      </c>
+      <c r="D77">
+        <v>4759</v>
+      </c>
+      <c r="E77">
+        <v>7.1</v>
+      </c>
+      <c r="F77">
+        <v>31912</v>
+      </c>
+      <c r="G77">
+        <v>2</v>
+      </c>
+      <c r="H77">
+        <v>4</v>
+      </c>
+      <c r="I77">
+        <v>40982</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>12</v>
+      </c>
+      <c r="B78" t="s">
+        <v>40</v>
+      </c>
+      <c r="C78" t="s">
+        <v>38</v>
+      </c>
+      <c r="D78">
+        <v>4759</v>
+      </c>
+      <c r="E78">
+        <v>7.1</v>
+      </c>
+      <c r="F78">
+        <v>31601</v>
+      </c>
+      <c r="G78">
+        <v>4</v>
+      </c>
+      <c r="H78">
+        <v>2</v>
+      </c>
+      <c r="I78">
+        <v>37607</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>12</v>
+      </c>
+      <c r="B79" t="s">
+        <v>38</v>
+      </c>
+      <c r="C79" t="s">
+        <v>39</v>
+      </c>
+      <c r="D79">
+        <v>3931</v>
+      </c>
+      <c r="E79">
+        <v>6</v>
+      </c>
+      <c r="F79">
+        <v>26678</v>
+      </c>
+      <c r="G79">
+        <v>2</v>
+      </c>
+      <c r="H79">
+        <v>5</v>
+      </c>
+      <c r="I79">
+        <v>47765</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>12</v>
+      </c>
+      <c r="B80" t="s">
+        <v>39</v>
+      </c>
+      <c r="C80" t="s">
+        <v>38</v>
+      </c>
+      <c r="D80">
+        <v>3931</v>
+      </c>
+      <c r="E80">
+        <v>6</v>
+      </c>
+      <c r="F80">
+        <v>26542</v>
+      </c>
+      <c r="G80">
+        <v>5</v>
+      </c>
+      <c r="H80">
+        <v>2</v>
+      </c>
+      <c r="I80">
+        <v>46553</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>12</v>
+      </c>
+      <c r="B81" t="s">
+        <v>38</v>
+      </c>
+      <c r="C81" t="s">
+        <v>40</v>
+      </c>
+      <c r="D81">
+        <v>4759</v>
+      </c>
+      <c r="E81">
+        <v>7.1</v>
+      </c>
+      <c r="F81">
+        <v>31912</v>
+      </c>
+      <c r="G81">
+        <v>2</v>
+      </c>
+      <c r="H81">
+        <v>4</v>
+      </c>
+      <c r="I81">
+        <v>40982</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>12</v>
+      </c>
+      <c r="B82" t="s">
+        <v>40</v>
+      </c>
+      <c r="C82" t="s">
+        <v>38</v>
+      </c>
+      <c r="D82">
+        <v>4759</v>
+      </c>
+      <c r="E82">
+        <v>7.1</v>
+      </c>
+      <c r="F82">
+        <v>31601</v>
+      </c>
+      <c r="G82">
+        <v>4</v>
+      </c>
+      <c r="H82">
+        <v>2</v>
+      </c>
+      <c r="I82">
+        <v>37607</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>12</v>
+      </c>
+      <c r="B83" t="s">
+        <v>38</v>
+      </c>
+      <c r="C83" t="s">
+        <v>60</v>
+      </c>
+      <c r="D83">
+        <v>2400</v>
+      </c>
+      <c r="E83">
+        <v>3.8</v>
+      </c>
+      <c r="F83">
+        <v>17325</v>
+      </c>
+      <c r="G83">
+        <v>2</v>
+      </c>
+      <c r="H83">
+        <v>3</v>
+      </c>
+      <c r="I83">
+        <v>47148</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>12</v>
+      </c>
+      <c r="B84" t="s">
+        <v>60</v>
+      </c>
+      <c r="C84" t="s">
+        <v>61</v>
+      </c>
+      <c r="D84">
+        <v>2097</v>
+      </c>
+      <c r="E84">
+        <v>3.4</v>
+      </c>
+      <c r="F84">
+        <v>15401</v>
+      </c>
+      <c r="G84">
+        <v>3</v>
+      </c>
+      <c r="H84">
+        <v>2</v>
+      </c>
+      <c r="I84">
+        <v>48747</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>12</v>
+      </c>
+      <c r="B85" t="s">
+        <v>61</v>
+      </c>
+      <c r="C85" t="s">
+        <v>38</v>
+      </c>
+      <c r="D85">
+        <v>1186</v>
+      </c>
+      <c r="E85">
+        <v>2.1</v>
+      </c>
+      <c r="F85">
+        <v>9765</v>
+      </c>
+      <c r="G85">
+        <v>2</v>
+      </c>
+      <c r="H85">
+        <v>2</v>
+      </c>
+      <c r="I85">
+        <v>46386</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>12</v>
+      </c>
+      <c r="B86" t="s">
+        <v>38</v>
+      </c>
+      <c r="C86" t="s">
+        <v>55</v>
+      </c>
+      <c r="D86">
+        <v>1950</v>
+      </c>
+      <c r="E86">
+        <v>3.2</v>
+      </c>
+      <c r="F86">
+        <v>14562</v>
+      </c>
+      <c r="G86">
+        <v>2</v>
+      </c>
+      <c r="H86">
+        <v>2</v>
+      </c>
+      <c r="I86">
+        <v>47462</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>12</v>
+      </c>
+      <c r="B87" t="s">
+        <v>55</v>
+      </c>
+      <c r="C87" t="s">
+        <v>56</v>
+      </c>
+      <c r="D87">
+        <v>181</v>
+      </c>
+      <c r="E87">
+        <v>0.8</v>
+      </c>
+      <c r="F87">
+        <v>3666</v>
+      </c>
+      <c r="G87">
+        <v>2</v>
+      </c>
+      <c r="H87">
+        <v>4</v>
+      </c>
+      <c r="I87">
+        <v>43984</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>12</v>
+      </c>
+      <c r="B88" t="s">
+        <v>56</v>
+      </c>
+      <c r="C88" t="s">
+        <v>38</v>
+      </c>
+      <c r="D88">
+        <v>1809</v>
+      </c>
+      <c r="E88">
+        <v>3</v>
+      </c>
+      <c r="F88">
+        <v>13568</v>
+      </c>
+      <c r="G88">
+        <v>4</v>
+      </c>
+      <c r="H88">
+        <v>2</v>
+      </c>
+      <c r="I88">
+        <v>41907</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>12</v>
+      </c>
+      <c r="B89" t="s">
+        <v>38</v>
+      </c>
+      <c r="C89" t="s">
+        <v>57</v>
+      </c>
+      <c r="D89">
+        <v>796</v>
+      </c>
+      <c r="E89">
+        <v>1.6</v>
+      </c>
+      <c r="F89">
+        <v>7395</v>
+      </c>
+      <c r="G89">
+        <v>2</v>
+      </c>
+      <c r="H89">
+        <v>3</v>
+      </c>
+      <c r="I89">
+        <v>45199</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>12</v>
+      </c>
+      <c r="B90" t="s">
+        <v>57</v>
+      </c>
+      <c r="C90" t="s">
+        <v>58</v>
+      </c>
+      <c r="D90">
+        <v>880</v>
+      </c>
+      <c r="E90">
+        <v>1.7</v>
+      </c>
+      <c r="F90">
+        <v>7927</v>
+      </c>
+      <c r="G90">
+        <v>3</v>
+      </c>
+      <c r="H90">
+        <v>2</v>
+      </c>
+      <c r="I90">
+        <v>43359</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>12</v>
+      </c>
+      <c r="B91" t="s">
+        <v>58</v>
+      </c>
+      <c r="C91" t="s">
+        <v>59</v>
+      </c>
+      <c r="D91">
+        <v>200</v>
+      </c>
+      <c r="E91">
+        <v>0.8</v>
+      </c>
+      <c r="F91">
+        <v>3818</v>
+      </c>
+      <c r="G91">
+        <v>2</v>
+      </c>
+      <c r="H91">
+        <v>5</v>
+      </c>
+      <c r="I91">
+        <v>41287</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>12</v>
+      </c>
+      <c r="B92" t="s">
+        <v>59</v>
+      </c>
+      <c r="C92" t="s">
+        <v>38</v>
+      </c>
+      <c r="D92">
+        <v>1504</v>
+      </c>
+      <c r="E92">
+        <v>2.6</v>
+      </c>
+      <c r="F92">
+        <v>11708</v>
+      </c>
+      <c r="G92">
+        <v>5</v>
+      </c>
+      <c r="H92">
+        <v>2</v>
+      </c>
+      <c r="I92">
+        <v>41972</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>12</v>
+      </c>
+      <c r="B93" t="s">
+        <v>38</v>
+      </c>
+      <c r="C93" t="s">
+        <v>57</v>
+      </c>
+      <c r="D93">
+        <v>796</v>
+      </c>
+      <c r="E93">
+        <v>1.6</v>
+      </c>
+      <c r="F93">
+        <v>7395</v>
+      </c>
+      <c r="G93">
+        <v>2</v>
+      </c>
+      <c r="H93">
+        <v>3</v>
+      </c>
+      <c r="I93">
+        <v>45199</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>12</v>
+      </c>
+      <c r="B94" t="s">
+        <v>57</v>
+      </c>
+      <c r="C94" t="s">
+        <v>58</v>
+      </c>
+      <c r="D94">
+        <v>880</v>
+      </c>
+      <c r="E94">
+        <v>1.7</v>
+      </c>
+      <c r="F94">
+        <v>7927</v>
+      </c>
+      <c r="G94">
+        <v>3</v>
+      </c>
+      <c r="H94">
+        <v>3</v>
+      </c>
+      <c r="I94">
+        <v>43359</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>12</v>
+      </c>
+      <c r="B95" t="s">
+        <v>58</v>
+      </c>
+      <c r="C95" t="s">
+        <v>59</v>
+      </c>
+      <c r="D95">
+        <v>200</v>
+      </c>
+      <c r="E95">
+        <v>0.8</v>
+      </c>
+      <c r="F95">
+        <v>3818</v>
+      </c>
+      <c r="G95">
+        <v>3</v>
+      </c>
+      <c r="H95">
+        <v>5</v>
+      </c>
+      <c r="I95">
+        <v>41287</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>12</v>
+      </c>
+      <c r="B96" t="s">
+        <v>59</v>
+      </c>
+      <c r="C96" t="s">
+        <v>38</v>
+      </c>
+      <c r="D96">
+        <v>1504</v>
+      </c>
+      <c r="E96">
+        <v>2.6</v>
+      </c>
+      <c r="F96">
+        <v>11708</v>
+      </c>
+      <c r="G96">
+        <v>5</v>
+      </c>
+      <c r="H96">
+        <v>2</v>
+      </c>
+      <c r="I96">
+        <v>41972</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>12</v>
+      </c>
+      <c r="B97" t="s">
+        <v>38</v>
+      </c>
+      <c r="C97" t="s">
+        <v>65</v>
+      </c>
+      <c r="D97">
+        <v>2171</v>
+      </c>
+      <c r="E97">
+        <v>3.5</v>
+      </c>
+      <c r="F97">
+        <v>15594</v>
+      </c>
+      <c r="G97">
+        <v>2</v>
+      </c>
+      <c r="H97">
+        <v>5</v>
+      </c>
+      <c r="I97">
+        <v>6861</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>12</v>
+      </c>
+      <c r="B98" t="s">
+        <v>65</v>
+      </c>
+      <c r="C98" t="s">
+        <v>66</v>
+      </c>
+      <c r="D98">
+        <v>4103</v>
+      </c>
+      <c r="E98">
+        <v>6.2</v>
+      </c>
+      <c r="F98">
+        <v>27805</v>
+      </c>
+      <c r="G98">
+        <v>5</v>
+      </c>
+      <c r="H98">
+        <v>5</v>
+      </c>
+      <c r="I98">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>12</v>
+      </c>
+      <c r="B99" t="s">
+        <v>66</v>
+      </c>
+      <c r="C99" t="s">
+        <v>67</v>
+      </c>
+      <c r="D99">
+        <v>3621</v>
+      </c>
+      <c r="E99">
+        <v>5.5</v>
+      </c>
+      <c r="F99">
+        <v>24668</v>
+      </c>
+      <c r="G99">
+        <v>5</v>
+      </c>
+      <c r="H99">
+        <v>5</v>
+      </c>
+      <c r="I99">
+        <v>41072</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>80</v>
+      </c>
+      <c r="B100" t="s">
+        <v>41</v>
+      </c>
+      <c r="C100" t="s">
+        <v>38</v>
+      </c>
+      <c r="D100">
+        <v>51</v>
+      </c>
+      <c r="E100">
+        <v>0.7</v>
+      </c>
+      <c r="F100">
+        <v>22</v>
+      </c>
+      <c r="G100">
+        <v>5</v>
+      </c>
+      <c r="H100">
+        <v>2</v>
+      </c>
+      <c r="I100">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>80</v>
+      </c>
+      <c r="B101" t="s">
+        <v>38</v>
+      </c>
+      <c r="C101" t="s">
+        <v>81</v>
+      </c>
+      <c r="D101">
+        <v>556</v>
+      </c>
+      <c r="E101">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="F101">
+        <v>64</v>
+      </c>
+      <c r="G101">
+        <v>2</v>
+      </c>
+      <c r="H101">
+        <v>4</v>
+      </c>
+      <c r="I101">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>80</v>
+      </c>
+      <c r="B102" t="s">
+        <v>81</v>
+      </c>
+      <c r="C102" t="s">
+        <v>76</v>
+      </c>
+      <c r="D102">
+        <v>565</v>
+      </c>
+      <c r="E102">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="F102">
+        <v>61</v>
+      </c>
+      <c r="G102">
+        <v>4</v>
+      </c>
+      <c r="H102">
+        <v>4</v>
+      </c>
+      <c r="I102">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>80</v>
+      </c>
+      <c r="B103" t="s">
+        <v>76</v>
+      </c>
+      <c r="C103" t="s">
+        <v>96</v>
+      </c>
+      <c r="D103">
+        <v>931</v>
+      </c>
+      <c r="E103">
+        <v>3.4</v>
+      </c>
+      <c r="F103">
+        <v>96</v>
+      </c>
+      <c r="G103">
+        <v>4</v>
+      </c>
+      <c r="H103">
+        <v>4</v>
+      </c>
+      <c r="I103">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>80</v>
+      </c>
+      <c r="B104" t="s">
+        <v>76</v>
+      </c>
+      <c r="C104" t="s">
+        <v>97</v>
+      </c>
+      <c r="D104">
+        <v>781</v>
+      </c>
+      <c r="E104">
+        <v>2.9</v>
+      </c>
+      <c r="F104">
+        <v>83</v>
+      </c>
+      <c r="G104">
+        <v>4</v>
+      </c>
+      <c r="H104">
+        <v>4</v>
+      </c>
+      <c r="I104">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>80</v>
+      </c>
+      <c r="B105" t="s">
+        <v>97</v>
+      </c>
+      <c r="C105" t="s">
+        <v>41</v>
+      </c>
+      <c r="D105">
+        <v>395</v>
+      </c>
+      <c r="E105">
+        <v>1.7</v>
+      </c>
+      <c r="F105">
+        <v>61</v>
+      </c>
+      <c r="G105">
+        <v>4</v>
+      </c>
+      <c r="H105">
+        <v>5</v>
+      </c>
+      <c r="I105">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>14</v>
+      </c>
+      <c r="B106" t="s">
+        <v>41</v>
+      </c>
+      <c r="C106" t="s">
+        <v>98</v>
+      </c>
+      <c r="D106">
+        <v>1752</v>
+      </c>
+      <c r="E106">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="F106">
+        <v>860</v>
+      </c>
+      <c r="G106">
+        <v>5</v>
+      </c>
+      <c r="H106">
+        <v>5</v>
+      </c>
+      <c r="I106">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>14</v>
+      </c>
+      <c r="B107" t="s">
+        <v>41</v>
+      </c>
+      <c r="C107" t="s">
+        <v>49</v>
+      </c>
+      <c r="D107">
+        <v>36</v>
+      </c>
+      <c r="E107">
+        <v>0.5</v>
+      </c>
+      <c r="F107">
+        <v>230</v>
+      </c>
+      <c r="G107">
+        <v>5</v>
+      </c>
+      <c r="H107">
+        <v>1</v>
+      </c>
+      <c r="I107">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>14</v>
+      </c>
+      <c r="B108" t="s">
+        <v>41</v>
+      </c>
+      <c r="C108" t="s">
+        <v>73</v>
+      </c>
+      <c r="D108">
+        <v>742</v>
+      </c>
+      <c r="E108">
+        <v>1.2</v>
+      </c>
+      <c r="F108">
+        <v>484</v>
+      </c>
+      <c r="G108">
+        <v>5</v>
+      </c>
+      <c r="H108">
+        <v>5</v>
+      </c>
+      <c r="I108">
+        <v>8355</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I47">
-    <sortCondition ref="A2:A47"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I102">
+    <sortCondition ref="A2:A102"/>
   </sortState>
+  <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Export: reorder columns, remove plane_id; show FBO ICAO in source; truncate job_id to 5; update Excel/CSV headers and formatting
</commit_message>
<xml_diff>
--- a/planes.xlsx
+++ b/planes.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aaron\OnAir\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aaron\Documents\GitHub\OnAirWorkOrders\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8783EE2A-A1F9-44DD-ACA6-266E5AA4DBDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ADD823F-A900-4630-8402-94FDF31B035F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{7DA1CCB9-1292-47D3-ABC3-3EB19435A409}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="115">
   <si>
     <t>Plane</t>
   </si>
@@ -331,6 +331,54 @@
   </si>
   <si>
     <t>TFFR</t>
+  </si>
+  <si>
+    <t>Smaug</t>
+  </si>
+  <si>
+    <t>CYHZ</t>
+  </si>
+  <si>
+    <t>KMHT</t>
+  </si>
+  <si>
+    <t>CYRQ</t>
+  </si>
+  <si>
+    <t>KELM</t>
+  </si>
+  <si>
+    <t>KFOK</t>
+  </si>
+  <si>
+    <t>CYFC</t>
+  </si>
+  <si>
+    <t>CYQB</t>
+  </si>
+  <si>
+    <t>C208 Grand Caravan Amphibian</t>
+  </si>
+  <si>
+    <t>KPBG</t>
+  </si>
+  <si>
+    <t>WYTOP</t>
+  </si>
+  <si>
+    <t>CYSC</t>
+  </si>
+  <si>
+    <t>CYDF</t>
+  </si>
+  <si>
+    <t>KROW</t>
+  </si>
+  <si>
+    <t>KPIH</t>
+  </si>
+  <si>
+    <t>KBXM</t>
   </si>
 </sst>
 </file>
@@ -1197,15 +1245,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A16643A-B77F-44B3-83CF-168AF5426912}">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1"/>
@@ -1273,25 +1321,25 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>107</v>
       </c>
       <c r="B3">
-        <v>414</v>
+        <v>186</v>
       </c>
       <c r="C3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D3">
-        <v>4271</v>
+        <v>887</v>
       </c>
       <c r="E3">
-        <v>38702</v>
+        <v>1430</v>
       </c>
       <c r="F3">
-        <v>369</v>
+        <v>3</v>
       </c>
       <c r="G3">
-        <v>135732</v>
+        <v>3435</v>
       </c>
       <c r="H3" t="s">
         <v>9</v>
@@ -1302,28 +1350,28 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B4">
-        <v>721</v>
+        <v>414</v>
       </c>
       <c r="C4">
         <v>2</v>
       </c>
       <c r="D4">
-        <v>6118</v>
+        <v>4271</v>
       </c>
       <c r="E4">
-        <v>19663</v>
+        <v>38702</v>
       </c>
       <c r="F4">
-        <v>5378</v>
+        <v>369</v>
       </c>
       <c r="G4">
-        <v>49936</v>
+        <v>135732</v>
       </c>
       <c r="H4" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="I4" t="s">
         <v>19</v>
@@ -1331,28 +1379,28 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>77</v>
       </c>
       <c r="B5">
-        <v>1165</v>
+        <v>483</v>
       </c>
       <c r="C5">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D5">
-        <v>3318</v>
+        <v>3259</v>
       </c>
       <c r="E5">
-        <v>30249</v>
+        <v>1574</v>
       </c>
       <c r="F5">
-        <v>3292</v>
+        <v>2829</v>
       </c>
       <c r="G5">
-        <v>31640</v>
+        <v>3346</v>
       </c>
       <c r="H5" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="I5" t="s">
         <v>19</v>
@@ -1360,25 +1408,25 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B6">
-        <v>999</v>
+        <v>1165</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D6">
-        <v>1806</v>
+        <v>3318</v>
       </c>
       <c r="E6">
-        <v>9390</v>
+        <v>30249</v>
       </c>
       <c r="F6">
-        <v>114</v>
+        <v>3292</v>
       </c>
       <c r="G6">
-        <v>13620</v>
+        <v>31640</v>
       </c>
       <c r="H6" t="s">
         <v>15</v>
@@ -1389,108 +1437,198 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B7">
-        <v>1910</v>
+        <v>150</v>
       </c>
       <c r="C7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D7">
-        <v>1869</v>
+        <v>2532</v>
       </c>
       <c r="E7">
-        <v>83</v>
+        <v>93225</v>
       </c>
       <c r="F7">
-        <v>1869</v>
+        <v>1350</v>
       </c>
       <c r="G7">
-        <v>83</v>
+        <v>109872</v>
       </c>
       <c r="H7" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="I7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B8">
-        <v>150</v>
+        <v>1910</v>
       </c>
       <c r="C8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D8">
-        <v>2532</v>
+        <v>1869</v>
       </c>
       <c r="E8">
-        <v>93225</v>
+        <v>83</v>
       </c>
       <c r="F8">
-        <v>1350</v>
+        <v>1869</v>
       </c>
       <c r="G8">
-        <v>109872</v>
+        <v>83</v>
       </c>
       <c r="H8" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="I8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>80</v>
+        <v>12</v>
       </c>
       <c r="B9">
-        <v>320</v>
+        <v>721</v>
       </c>
       <c r="C9">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D9">
-        <v>1044</v>
+        <v>6118</v>
       </c>
       <c r="E9">
-        <v>219</v>
+        <v>19663</v>
       </c>
       <c r="F9">
-        <v>1</v>
+        <v>5378</v>
       </c>
       <c r="G9">
-        <v>800</v>
+        <v>49936</v>
       </c>
       <c r="H9" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="I9" t="s">
         <v>19</v>
       </c>
     </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>99</v>
+      </c>
+      <c r="B10">
+        <v>160</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>572</v>
+      </c>
+      <c r="E10">
+        <v>338</v>
+      </c>
+      <c r="F10">
+        <v>15</v>
+      </c>
+      <c r="G10">
+        <v>1250</v>
+      </c>
+      <c r="H10" t="s">
+        <v>9</v>
+      </c>
+      <c r="I10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>80</v>
+      </c>
+      <c r="B11">
+        <v>320</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>1044</v>
+      </c>
+      <c r="E11">
+        <v>219</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11">
+        <v>800</v>
+      </c>
+      <c r="H11" t="s">
+        <v>9</v>
+      </c>
+      <c r="I11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12">
+        <v>999</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>1806</v>
+      </c>
+      <c r="E12">
+        <v>9390</v>
+      </c>
+      <c r="F12">
+        <v>114</v>
+      </c>
+      <c r="G12">
+        <v>13620</v>
+      </c>
+      <c r="H12" t="s">
+        <v>15</v>
+      </c>
+      <c r="I12" t="s">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I12">
+    <sortCondition ref="A2:A12"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B22E5411-C937-41B5-8075-5A67875F9274}">
-  <dimension ref="A1:I108"/>
+  <dimension ref="A1:I151"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A108" sqref="A108"/>
+      <pane ySplit="1" topLeftCell="A128" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A149" sqref="A149"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.7109375" bestFit="1" customWidth="1"/>
@@ -2488,202 +2626,202 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>10</v>
+        <v>107</v>
       </c>
       <c r="B35" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="C35" t="s">
-        <v>62</v>
+        <v>106</v>
       </c>
       <c r="D35">
-        <v>2876</v>
+        <v>147</v>
       </c>
       <c r="E35">
-        <v>7.4</v>
+        <v>1.3</v>
       </c>
       <c r="F35">
-        <v>12280</v>
+        <v>101</v>
       </c>
       <c r="G35">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="H35">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I35">
-        <v>91473</v>
+        <v>64</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>10</v>
+        <v>107</v>
       </c>
       <c r="B36" t="s">
-        <v>62</v>
+        <v>106</v>
       </c>
       <c r="C36" t="s">
-        <v>37</v>
+        <v>108</v>
       </c>
       <c r="D36">
-        <v>2932</v>
+        <v>155</v>
       </c>
       <c r="E36">
-        <v>7.6</v>
+        <v>1.3</v>
       </c>
       <c r="F36">
-        <v>11845</v>
+        <v>101</v>
       </c>
       <c r="G36">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H36">
         <v>5</v>
       </c>
       <c r="I36">
-        <v>64040</v>
+        <v>22</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>10</v>
+        <v>107</v>
       </c>
       <c r="B37" t="s">
-        <v>37</v>
+        <v>108</v>
       </c>
       <c r="C37" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
       <c r="D37">
-        <v>573</v>
+        <v>214</v>
       </c>
       <c r="E37">
-        <v>1.9</v>
+        <v>1.6</v>
       </c>
       <c r="F37">
-        <v>3164</v>
+        <v>132</v>
       </c>
       <c r="G37">
         <v>5</v>
       </c>
       <c r="H37">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I37">
-        <v>20465</v>
+        <v>36</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>10</v>
+        <v>107</v>
       </c>
       <c r="B38" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
       <c r="C38" t="s">
-        <v>64</v>
+        <v>109</v>
       </c>
       <c r="D38">
-        <v>73</v>
+        <v>30</v>
       </c>
       <c r="E38">
         <v>0.7</v>
       </c>
       <c r="F38">
-        <v>1242</v>
+        <v>60</v>
       </c>
       <c r="G38">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="H38">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="I38">
-        <v>95123</v>
+        <v>1543</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>10</v>
+        <v>107</v>
       </c>
       <c r="B39" t="s">
-        <v>64</v>
+        <v>109</v>
       </c>
       <c r="C39" t="s">
-        <v>29</v>
+        <v>110</v>
       </c>
       <c r="D39">
-        <v>926</v>
+        <v>150</v>
       </c>
       <c r="E39">
-        <v>2.7</v>
+        <v>1.3</v>
       </c>
       <c r="F39">
-        <v>4440</v>
+        <v>105</v>
       </c>
       <c r="G39">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H39">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="I39">
-        <v>91473</v>
+        <v>645</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>10</v>
+        <v>107</v>
       </c>
       <c r="B40" t="s">
-        <v>29</v>
+        <v>110</v>
       </c>
       <c r="C40" t="s">
-        <v>41</v>
+        <v>109</v>
       </c>
       <c r="D40">
-        <v>1604</v>
+        <v>150</v>
       </c>
       <c r="E40">
-        <v>4.4000000000000004</v>
+        <v>1.3</v>
       </c>
       <c r="F40">
-        <v>7367</v>
+        <v>101</v>
       </c>
       <c r="G40">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="H40">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="I40">
-        <v>0</v>
+        <v>596</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>77</v>
+        <v>107</v>
       </c>
       <c r="B41" t="s">
-        <v>41</v>
+        <v>109</v>
       </c>
       <c r="C41" t="s">
-        <v>78</v>
+        <v>111</v>
       </c>
       <c r="D41">
-        <v>508</v>
+        <v>481</v>
       </c>
       <c r="E41">
-        <v>1.6</v>
+        <v>3.1</v>
       </c>
       <c r="F41">
-        <v>477</v>
+        <v>215</v>
       </c>
       <c r="G41">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H41">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I41">
         <v>0</v>
@@ -2691,283 +2829,283 @@
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>77</v>
+        <v>107</v>
       </c>
       <c r="B42" t="s">
-        <v>78</v>
+        <v>111</v>
       </c>
       <c r="C42" t="s">
-        <v>79</v>
+        <v>49</v>
       </c>
       <c r="D42">
-        <v>2849</v>
+        <v>508</v>
       </c>
       <c r="E42">
-        <v>6.4</v>
+        <v>3.2</v>
       </c>
       <c r="F42">
-        <v>1972</v>
+        <v>231</v>
       </c>
       <c r="G42">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H42">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I42">
-        <v>1863</v>
+        <v>25</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>13</v>
+        <v>107</v>
       </c>
       <c r="B43" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="C43" t="s">
-        <v>42</v>
+        <v>111</v>
       </c>
       <c r="D43">
-        <v>1983</v>
+        <v>508</v>
       </c>
       <c r="E43">
-        <v>2.2000000000000002</v>
+        <v>3.2</v>
       </c>
       <c r="F43">
-        <v>21251</v>
+        <v>224</v>
       </c>
       <c r="G43">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="H43">
         <v>4</v>
       </c>
       <c r="I43">
-        <v>12106</v>
+        <v>23</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>13</v>
+        <v>107</v>
       </c>
       <c r="B44" t="s">
-        <v>42</v>
+        <v>111</v>
       </c>
       <c r="C44" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D44">
-        <v>1548</v>
+        <v>536</v>
       </c>
       <c r="E44">
-        <v>1.8</v>
+        <v>3.4</v>
       </c>
       <c r="F44">
-        <v>17679</v>
+        <v>272</v>
       </c>
       <c r="G44">
         <v>4</v>
       </c>
       <c r="H44">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I44">
-        <v>3318</v>
+        <v>1585</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B45" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C45" t="s">
-        <v>44</v>
+        <v>62</v>
       </c>
       <c r="D45">
-        <v>415</v>
+        <v>2876</v>
       </c>
       <c r="E45">
-        <v>0.9</v>
+        <v>7.4</v>
       </c>
       <c r="F45">
-        <v>8443</v>
+        <v>12280</v>
       </c>
       <c r="G45">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H45">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I45">
-        <v>25201</v>
+        <v>91473</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B46" t="s">
-        <v>44</v>
+        <v>62</v>
       </c>
       <c r="C46" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="D46">
-        <v>1954</v>
+        <v>2932</v>
       </c>
       <c r="E46">
-        <v>2.2000000000000002</v>
+        <v>7.6</v>
       </c>
       <c r="F46">
-        <v>20857</v>
+        <v>11845</v>
       </c>
       <c r="G46">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H46">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I46">
-        <v>22586</v>
+        <v>64040</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B47" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="C47" t="s">
-        <v>41</v>
+        <v>63</v>
       </c>
       <c r="D47">
-        <v>3037</v>
+        <v>573</v>
       </c>
       <c r="E47">
-        <v>3.1</v>
+        <v>1.9</v>
       </c>
       <c r="F47">
-        <v>30551</v>
+        <v>3164</v>
       </c>
       <c r="G47">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H47">
         <v>5</v>
       </c>
       <c r="I47">
-        <v>19837</v>
+        <v>20465</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B48" t="s">
-        <v>41</v>
+        <v>63</v>
       </c>
       <c r="C48" t="s">
-        <v>46</v>
+        <v>64</v>
       </c>
       <c r="D48">
-        <v>2727</v>
+        <v>73</v>
       </c>
       <c r="E48">
-        <v>2.8</v>
+        <v>0.7</v>
       </c>
       <c r="F48">
-        <v>27806</v>
+        <v>1242</v>
       </c>
       <c r="G48">
         <v>5</v>
       </c>
       <c r="H48">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I48">
-        <v>9758</v>
+        <v>95123</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B49" t="s">
-        <v>46</v>
+        <v>64</v>
       </c>
       <c r="C49" t="s">
-        <v>47</v>
+        <v>29</v>
       </c>
       <c r="D49">
-        <v>2034</v>
+        <v>926</v>
       </c>
       <c r="E49">
-        <v>2.2000000000000002</v>
+        <v>2.7</v>
       </c>
       <c r="F49">
-        <v>24970</v>
+        <v>4440</v>
       </c>
       <c r="G49">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H49">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I49">
-        <v>14131</v>
+        <v>91473</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B50" t="s">
-        <v>47</v>
+        <v>29</v>
       </c>
       <c r="C50" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="D50">
-        <v>1100</v>
+        <v>1604</v>
       </c>
       <c r="E50">
-        <v>1.4</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="F50">
-        <v>14081</v>
+        <v>7367</v>
       </c>
       <c r="G50">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H50">
         <v>5</v>
       </c>
       <c r="I50">
-        <v>27903</v>
+        <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>13</v>
+        <v>77</v>
       </c>
       <c r="B51" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="C51" t="s">
-        <v>41</v>
+        <v>78</v>
       </c>
       <c r="D51">
-        <v>226</v>
+        <v>508</v>
       </c>
       <c r="E51">
-        <v>0.7</v>
+        <v>1.6</v>
       </c>
       <c r="F51">
-        <v>7917</v>
+        <v>477</v>
       </c>
       <c r="G51">
         <v>5</v>
@@ -2976,85 +3114,85 @@
         <v>5</v>
       </c>
       <c r="I51">
-        <v>31131</v>
+        <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>13</v>
+        <v>77</v>
       </c>
       <c r="B52" t="s">
-        <v>41</v>
+        <v>78</v>
       </c>
       <c r="C52" t="s">
-        <v>68</v>
+        <v>79</v>
       </c>
       <c r="D52">
-        <v>1581</v>
+        <v>2849</v>
       </c>
       <c r="E52">
-        <v>1.9</v>
+        <v>6.4</v>
       </c>
       <c r="F52">
-        <v>18239</v>
+        <v>1972</v>
       </c>
       <c r="G52">
         <v>5</v>
       </c>
       <c r="H52">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I52">
-        <v>562</v>
+        <v>1863</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>13</v>
+        <v>77</v>
       </c>
       <c r="B53" t="s">
-        <v>68</v>
+        <v>49</v>
       </c>
       <c r="C53" t="s">
-        <v>41</v>
+        <v>112</v>
       </c>
       <c r="D53">
-        <v>1581</v>
+        <v>1802</v>
       </c>
       <c r="E53">
-        <v>1.9</v>
+        <v>4.2</v>
       </c>
       <c r="F53">
-        <v>18827</v>
+        <v>1292</v>
       </c>
       <c r="G53">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H53">
         <v>5</v>
       </c>
       <c r="I53">
-        <v>526</v>
+        <v>10</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>13</v>
+        <v>77</v>
       </c>
       <c r="B54" t="s">
-        <v>41</v>
+        <v>112</v>
       </c>
       <c r="C54" t="s">
-        <v>69</v>
+        <v>108</v>
       </c>
       <c r="D54">
-        <v>225</v>
+        <v>1588</v>
       </c>
       <c r="E54">
-        <v>0.7</v>
+        <v>3.8</v>
       </c>
       <c r="F54">
-        <v>6997</v>
+        <v>1160</v>
       </c>
       <c r="G54">
         <v>5</v>
@@ -3063,210 +3201,210 @@
         <v>5</v>
       </c>
       <c r="I54">
-        <v>29652</v>
+        <v>73</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>13</v>
+        <v>77</v>
       </c>
       <c r="B55" t="s">
-        <v>69</v>
+        <v>108</v>
       </c>
       <c r="C55" t="s">
-        <v>70</v>
+        <v>49</v>
       </c>
       <c r="D55">
-        <v>899</v>
+        <v>214</v>
       </c>
       <c r="E55">
-        <v>1.3</v>
+        <v>0.9</v>
       </c>
       <c r="F55">
-        <v>12440</v>
+        <v>332</v>
       </c>
       <c r="G55">
         <v>5</v>
       </c>
       <c r="H55">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I55">
-        <v>2732</v>
+        <v>40</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>13</v>
+        <v>77</v>
       </c>
       <c r="B56" t="s">
-        <v>70</v>
+        <v>49</v>
       </c>
       <c r="C56" t="s">
-        <v>41</v>
+        <v>95</v>
       </c>
       <c r="D56">
-        <v>1123</v>
+        <v>209</v>
       </c>
       <c r="E56">
-        <v>1.5</v>
+        <v>0.9</v>
       </c>
       <c r="F56">
-        <v>15139</v>
+        <v>302</v>
       </c>
       <c r="G56">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H56">
         <v>5</v>
       </c>
       <c r="I56">
-        <v>28914</v>
+        <v>40</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>13</v>
+        <v>77</v>
       </c>
       <c r="B57" t="s">
-        <v>41</v>
+        <v>95</v>
       </c>
       <c r="C57" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D57">
-        <v>975</v>
+        <v>69</v>
       </c>
       <c r="E57">
-        <v>1.3</v>
+        <v>0.6</v>
       </c>
       <c r="F57">
-        <v>13014</v>
+        <v>229</v>
       </c>
       <c r="G57">
         <v>5</v>
       </c>
       <c r="H57">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I57">
-        <v>9194</v>
+        <v>2</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>13</v>
+        <v>77</v>
       </c>
       <c r="B58" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C58" t="s">
-        <v>72</v>
+        <v>49</v>
       </c>
       <c r="D58">
-        <v>170</v>
+        <v>257</v>
       </c>
       <c r="E58">
-        <v>0.6</v>
+        <v>1</v>
       </c>
       <c r="F58">
-        <v>6142</v>
+        <v>358</v>
       </c>
       <c r="G58">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H58">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I58">
-        <v>12540</v>
+        <v>79</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>13</v>
+        <v>77</v>
       </c>
       <c r="B59" t="s">
-        <v>72</v>
+        <v>49</v>
       </c>
       <c r="C59" t="s">
-        <v>41</v>
+        <v>113</v>
       </c>
       <c r="D59">
-        <v>964</v>
+        <v>1879</v>
       </c>
       <c r="E59">
-        <v>1.3</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="F59">
-        <v>13856</v>
+        <v>1335</v>
       </c>
       <c r="G59">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="H59">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I59">
-        <v>2367</v>
+        <v>23</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>13</v>
+        <v>77</v>
       </c>
       <c r="B60" t="s">
-        <v>41</v>
+        <v>113</v>
       </c>
       <c r="C60" t="s">
-        <v>73</v>
+        <v>88</v>
       </c>
       <c r="D60">
-        <v>742</v>
+        <v>1196</v>
       </c>
       <c r="E60">
-        <v>1.1000000000000001</v>
+        <v>3</v>
       </c>
       <c r="F60">
-        <v>11106</v>
+        <v>917</v>
       </c>
       <c r="G60">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H60">
         <v>5</v>
       </c>
       <c r="I60">
-        <v>8355</v>
+        <v>4</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>13</v>
+        <v>77</v>
       </c>
       <c r="B61" t="s">
-        <v>73</v>
+        <v>88</v>
       </c>
       <c r="C61" t="s">
-        <v>74</v>
+        <v>49</v>
       </c>
       <c r="D61">
-        <v>339</v>
+        <v>853</v>
       </c>
       <c r="E61">
-        <v>0.8</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="F61">
-        <v>7935</v>
+        <v>726</v>
       </c>
       <c r="G61">
         <v>5</v>
       </c>
       <c r="H61">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I61">
-        <v>23387</v>
+        <v>18</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
@@ -3274,28 +3412,28 @@
         <v>13</v>
       </c>
       <c r="B62" t="s">
-        <v>74</v>
+        <v>41</v>
       </c>
       <c r="C62" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D62">
-        <v>1025</v>
+        <v>1983</v>
       </c>
       <c r="E62">
-        <v>1.4</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="F62">
-        <v>14348</v>
+        <v>21251</v>
       </c>
       <c r="G62">
         <v>5</v>
       </c>
       <c r="H62">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I62">
-        <v>12855</v>
+        <v>12106</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
@@ -3303,28 +3441,28 @@
         <v>13</v>
       </c>
       <c r="B63" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C63" t="s">
-        <v>75</v>
+        <v>43</v>
       </c>
       <c r="D63">
-        <v>1268</v>
+        <v>1548</v>
       </c>
       <c r="E63">
-        <v>1.6</v>
+        <v>1.8</v>
       </c>
       <c r="F63">
-        <v>15339</v>
+        <v>17679</v>
       </c>
       <c r="G63">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H63">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I63">
-        <v>0</v>
+        <v>3318</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
@@ -3332,28 +3470,28 @@
         <v>13</v>
       </c>
       <c r="B64" t="s">
-        <v>75</v>
+        <v>43</v>
       </c>
       <c r="C64" t="s">
-        <v>65</v>
+        <v>44</v>
       </c>
       <c r="D64">
-        <v>2363</v>
+        <v>415</v>
       </c>
       <c r="E64">
-        <v>2.5</v>
+        <v>0.9</v>
       </c>
       <c r="F64">
-        <v>23877</v>
+        <v>8443</v>
       </c>
       <c r="G64">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H64">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I64">
-        <v>13344</v>
+        <v>25201</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
@@ -3361,1280 +3499,2527 @@
         <v>13</v>
       </c>
       <c r="B65" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="C65" t="s">
-        <v>76</v>
+        <v>45</v>
       </c>
       <c r="D65">
-        <v>1051</v>
+        <v>1954</v>
       </c>
       <c r="E65">
-        <v>1.4</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="F65">
-        <v>13255</v>
+        <v>20857</v>
       </c>
       <c r="G65">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H65">
         <v>4</v>
       </c>
       <c r="I65">
-        <v>0</v>
+        <v>22586</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B66" t="s">
+        <v>45</v>
+      </c>
+      <c r="C66" t="s">
         <v>41</v>
       </c>
-      <c r="C66" t="s">
-        <v>38</v>
-      </c>
       <c r="D66">
-        <v>51</v>
+        <v>3037</v>
       </c>
       <c r="E66">
-        <v>0.8</v>
+        <v>3.1</v>
       </c>
       <c r="F66">
-        <v>415</v>
+        <v>30551</v>
       </c>
       <c r="G66">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H66">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="I66">
-        <v>0</v>
+        <v>19837</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B67" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C67" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D67">
-        <v>18</v>
+        <v>2727</v>
       </c>
       <c r="E67">
-        <v>0.6</v>
+        <v>2.8</v>
       </c>
       <c r="F67">
-        <v>412</v>
+        <v>27806</v>
       </c>
       <c r="G67">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H67">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I67">
-        <v>80278</v>
+        <v>9758</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B68" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C68" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="D68">
-        <v>36</v>
+        <v>2034</v>
       </c>
       <c r="E68">
-        <v>0.7</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="F68">
-        <v>669</v>
+        <v>24970</v>
       </c>
       <c r="G68">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H68">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I68">
-        <v>7393</v>
+        <v>14131</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B69" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C69" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D69">
-        <v>306</v>
+        <v>1100</v>
       </c>
       <c r="E69">
-        <v>0.7</v>
+        <v>1.4</v>
       </c>
       <c r="F69">
-        <v>6179</v>
+        <v>14081</v>
       </c>
       <c r="G69">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H69">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="I69">
-        <v>61</v>
+        <v>27903</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B70" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C70" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="D70">
-        <v>1084</v>
+        <v>226</v>
       </c>
       <c r="E70">
-        <v>1.1000000000000001</v>
+        <v>0.7</v>
       </c>
       <c r="F70">
-        <v>10949</v>
+        <v>7917</v>
       </c>
       <c r="G70">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H70">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I70">
-        <v>56</v>
+        <v>31131</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B71" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="C71" t="s">
-        <v>52</v>
+        <v>68</v>
       </c>
       <c r="D71">
-        <v>959</v>
+        <v>1581</v>
       </c>
       <c r="E71">
-        <v>1</v>
+        <v>1.9</v>
       </c>
       <c r="F71">
-        <v>11546</v>
+        <v>18239</v>
       </c>
       <c r="G71">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H71">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I71">
-        <v>31</v>
+        <v>562</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B72" t="s">
-        <v>49</v>
+        <v>68</v>
       </c>
       <c r="C72" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="D72">
-        <v>1716</v>
+        <v>1581</v>
       </c>
       <c r="E72">
-        <v>1.4</v>
+        <v>1.9</v>
       </c>
       <c r="F72">
-        <v>11721</v>
+        <v>18827</v>
       </c>
       <c r="G72">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H72">
         <v>5</v>
       </c>
       <c r="I72">
-        <v>52</v>
+        <v>526</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B73" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="C73" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="D73">
-        <v>528</v>
+        <v>225</v>
       </c>
       <c r="E73">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="F73">
-        <v>6601</v>
+        <v>6997</v>
       </c>
       <c r="G73">
         <v>5</v>
       </c>
       <c r="H73">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I73">
-        <v>67</v>
+        <v>29652</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B74" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="C74" t="s">
-        <v>49</v>
+        <v>70</v>
       </c>
       <c r="D74">
-        <v>1678</v>
+        <v>899</v>
       </c>
       <c r="E74">
-        <v>1.4</v>
+        <v>1.3</v>
       </c>
       <c r="F74">
-        <v>11520</v>
+        <v>12440</v>
       </c>
       <c r="G74">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H74">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I74">
-        <v>51</v>
+        <v>2732</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B75" t="s">
-        <v>38</v>
+        <v>70</v>
       </c>
       <c r="C75" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D75">
-        <v>3931</v>
+        <v>1123</v>
       </c>
       <c r="E75">
-        <v>6</v>
+        <v>1.5</v>
       </c>
       <c r="F75">
-        <v>26678</v>
+        <v>15139</v>
       </c>
       <c r="G75">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H75">
         <v>5</v>
       </c>
       <c r="I75">
-        <v>47765</v>
+        <v>28914</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B76" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C76" t="s">
-        <v>38</v>
+        <v>71</v>
       </c>
       <c r="D76">
-        <v>3931</v>
+        <v>975</v>
       </c>
       <c r="E76">
-        <v>6</v>
+        <v>1.3</v>
       </c>
       <c r="F76">
-        <v>26542</v>
+        <v>13014</v>
       </c>
       <c r="G76">
         <v>5</v>
       </c>
       <c r="H76">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I76">
-        <v>46553</v>
+        <v>9194</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B77" t="s">
-        <v>38</v>
+        <v>71</v>
       </c>
       <c r="C77" t="s">
-        <v>40</v>
+        <v>72</v>
       </c>
       <c r="D77">
-        <v>4759</v>
+        <v>170</v>
       </c>
       <c r="E77">
-        <v>7.1</v>
+        <v>0.6</v>
       </c>
       <c r="F77">
-        <v>31912</v>
+        <v>6142</v>
       </c>
       <c r="G77">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H77">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I77">
-        <v>40982</v>
+        <v>12540</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B78" t="s">
-        <v>40</v>
+        <v>72</v>
       </c>
       <c r="C78" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="D78">
-        <v>4759</v>
+        <v>964</v>
       </c>
       <c r="E78">
-        <v>7.1</v>
+        <v>1.3</v>
       </c>
       <c r="F78">
-        <v>31601</v>
+        <v>13856</v>
       </c>
       <c r="G78">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H78">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="I78">
-        <v>37607</v>
+        <v>2367</v>
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B79" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C79" t="s">
-        <v>39</v>
+        <v>73</v>
       </c>
       <c r="D79">
-        <v>3931</v>
+        <v>742</v>
       </c>
       <c r="E79">
-        <v>6</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="F79">
-        <v>26678</v>
+        <v>11106</v>
       </c>
       <c r="G79">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H79">
         <v>5</v>
       </c>
       <c r="I79">
-        <v>47765</v>
+        <v>8355</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B80" t="s">
-        <v>39</v>
+        <v>73</v>
       </c>
       <c r="C80" t="s">
-        <v>38</v>
+        <v>74</v>
       </c>
       <c r="D80">
-        <v>3931</v>
+        <v>339</v>
       </c>
       <c r="E80">
-        <v>6</v>
+        <v>0.8</v>
       </c>
       <c r="F80">
-        <v>26542</v>
+        <v>7935</v>
       </c>
       <c r="G80">
         <v>5</v>
       </c>
       <c r="H80">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="I80">
-        <v>46553</v>
+        <v>23387</v>
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B81" t="s">
-        <v>38</v>
+        <v>74</v>
       </c>
       <c r="C81" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D81">
-        <v>4759</v>
+        <v>1025</v>
       </c>
       <c r="E81">
-        <v>7.1</v>
+        <v>1.4</v>
       </c>
       <c r="F81">
-        <v>31912</v>
+        <v>14348</v>
       </c>
       <c r="G81">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H81">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I81">
-        <v>40982</v>
+        <v>12855</v>
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B82" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C82" t="s">
-        <v>38</v>
+        <v>75</v>
       </c>
       <c r="D82">
-        <v>4759</v>
+        <v>1268</v>
       </c>
       <c r="E82">
-        <v>7.1</v>
+        <v>1.6</v>
       </c>
       <c r="F82">
-        <v>31601</v>
+        <v>15339</v>
       </c>
       <c r="G82">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H82">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="I82">
-        <v>37607</v>
+        <v>0</v>
       </c>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B83" t="s">
-        <v>38</v>
+        <v>75</v>
       </c>
       <c r="C83" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="D83">
-        <v>2400</v>
+        <v>2363</v>
       </c>
       <c r="E83">
-        <v>3.8</v>
+        <v>2.5</v>
       </c>
       <c r="F83">
-        <v>17325</v>
+        <v>23877</v>
       </c>
       <c r="G83">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H83">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="I83">
-        <v>47148</v>
+        <v>13344</v>
       </c>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B84" t="s">
-        <v>60</v>
+        <v>41</v>
       </c>
       <c r="C84" t="s">
-        <v>61</v>
+        <v>76</v>
       </c>
       <c r="D84">
-        <v>2097</v>
+        <v>1051</v>
       </c>
       <c r="E84">
-        <v>3.4</v>
+        <v>1.4</v>
       </c>
       <c r="F84">
-        <v>15401</v>
+        <v>13255</v>
       </c>
       <c r="G84">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H84">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I84">
-        <v>48747</v>
+        <v>0</v>
       </c>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B85" t="s">
-        <v>61</v>
+        <v>41</v>
       </c>
       <c r="C85" t="s">
         <v>38</v>
       </c>
       <c r="D85">
-        <v>1186</v>
+        <v>51</v>
       </c>
       <c r="E85">
-        <v>2.1</v>
+        <v>0.8</v>
       </c>
       <c r="F85">
-        <v>9765</v>
+        <v>415</v>
       </c>
       <c r="G85">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H85">
         <v>2</v>
       </c>
       <c r="I85">
-        <v>46386</v>
+        <v>0</v>
       </c>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B86" t="s">
         <v>38</v>
       </c>
       <c r="C86" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="D86">
-        <v>1950</v>
+        <v>18</v>
       </c>
       <c r="E86">
-        <v>3.2</v>
+        <v>0.6</v>
       </c>
       <c r="F86">
-        <v>14562</v>
+        <v>412</v>
       </c>
       <c r="G86">
         <v>2</v>
       </c>
       <c r="H86">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I86">
-        <v>47462</v>
+        <v>80278</v>
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B87" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C87" t="s">
-        <v>56</v>
+        <v>41</v>
       </c>
       <c r="D87">
-        <v>181</v>
+        <v>36</v>
       </c>
       <c r="E87">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="F87">
-        <v>3666</v>
+        <v>669</v>
       </c>
       <c r="G87">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H87">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I87">
-        <v>43984</v>
+        <v>7393</v>
       </c>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B88" t="s">
-        <v>56</v>
+        <v>41</v>
       </c>
       <c r="C88" t="s">
         <v>38</v>
       </c>
       <c r="D88">
-        <v>1809</v>
+        <v>51</v>
       </c>
       <c r="E88">
-        <v>3</v>
+        <v>0.4</v>
       </c>
       <c r="F88">
-        <v>13568</v>
+        <v>415</v>
       </c>
       <c r="G88">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H88">
         <v>2</v>
       </c>
       <c r="I88">
-        <v>41907</v>
+        <v>0</v>
       </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B89" t="s">
         <v>38</v>
       </c>
       <c r="C89" t="s">
-        <v>57</v>
+        <v>94</v>
       </c>
       <c r="D89">
-        <v>796</v>
+        <v>382</v>
       </c>
       <c r="E89">
-        <v>1.6</v>
+        <v>3</v>
       </c>
       <c r="F89">
-        <v>7395</v>
+        <v>1115</v>
       </c>
       <c r="G89">
         <v>2</v>
       </c>
       <c r="H89">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="I89">
-        <v>45199</v>
+        <v>102957</v>
       </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B90" t="s">
-        <v>57</v>
+        <v>94</v>
       </c>
       <c r="C90" t="s">
-        <v>58</v>
+        <v>76</v>
       </c>
       <c r="D90">
-        <v>880</v>
+        <v>713</v>
       </c>
       <c r="E90">
-        <v>1.7</v>
+        <v>5.3</v>
       </c>
       <c r="F90">
-        <v>7927</v>
+        <v>1879</v>
       </c>
       <c r="G90">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H90">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I90">
-        <v>43359</v>
+        <v>73571</v>
       </c>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B91" t="s">
-        <v>58</v>
+        <v>76</v>
       </c>
       <c r="C91" t="s">
-        <v>59</v>
+        <v>75</v>
       </c>
       <c r="D91">
-        <v>200</v>
+        <v>291</v>
       </c>
       <c r="E91">
-        <v>0.8</v>
+        <v>2.4</v>
       </c>
       <c r="F91">
-        <v>3818</v>
+        <v>988</v>
       </c>
       <c r="G91">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H91">
         <v>5</v>
       </c>
       <c r="I91">
-        <v>41287</v>
+        <v>2300</v>
       </c>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B92" t="s">
-        <v>59</v>
+        <v>75</v>
       </c>
       <c r="C92" t="s">
-        <v>38</v>
+        <v>114</v>
       </c>
       <c r="D92">
-        <v>1504</v>
+        <v>1197</v>
       </c>
       <c r="E92">
-        <v>2.6</v>
+        <v>8.5</v>
       </c>
       <c r="F92">
-        <v>11708</v>
+        <v>3133</v>
       </c>
       <c r="G92">
         <v>5</v>
       </c>
       <c r="H92">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I92">
-        <v>41972</v>
+        <v>96431</v>
       </c>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B93" t="s">
-        <v>38</v>
+        <v>114</v>
       </c>
       <c r="C93" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="D93">
-        <v>796</v>
+        <v>73</v>
       </c>
       <c r="E93">
-        <v>1.6</v>
+        <v>1</v>
       </c>
       <c r="F93">
-        <v>7395</v>
+        <v>757</v>
       </c>
       <c r="G93">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H93">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="I93">
-        <v>45199</v>
+        <v>84021</v>
       </c>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B94" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="C94" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="D94">
-        <v>880</v>
+        <v>306</v>
       </c>
       <c r="E94">
-        <v>1.7</v>
+        <v>0.7</v>
       </c>
       <c r="F94">
-        <v>7927</v>
+        <v>6179</v>
       </c>
       <c r="G94">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H94">
         <v>3</v>
       </c>
       <c r="I94">
-        <v>43359</v>
+        <v>61</v>
       </c>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B95" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="C95" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="D95">
-        <v>200</v>
+        <v>1084</v>
       </c>
       <c r="E95">
-        <v>0.8</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="F95">
-        <v>3818</v>
+        <v>10949</v>
       </c>
       <c r="G95">
         <v>3</v>
       </c>
       <c r="H95">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I95">
-        <v>41287</v>
+        <v>56</v>
       </c>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B96" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="C96" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="D96">
-        <v>1504</v>
+        <v>959</v>
       </c>
       <c r="E96">
-        <v>2.6</v>
+        <v>1</v>
       </c>
       <c r="F96">
-        <v>11708</v>
+        <v>11546</v>
       </c>
       <c r="G96">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H96">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I96">
-        <v>41972</v>
+        <v>31</v>
       </c>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B97" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="C97" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="D97">
-        <v>2171</v>
+        <v>1716</v>
       </c>
       <c r="E97">
-        <v>3.5</v>
+        <v>1.4</v>
       </c>
       <c r="F97">
-        <v>15594</v>
+        <v>11721</v>
       </c>
       <c r="G97">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H97">
         <v>5</v>
       </c>
       <c r="I97">
-        <v>6861</v>
+        <v>52</v>
       </c>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B98" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="C98" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="D98">
-        <v>4103</v>
+        <v>528</v>
       </c>
       <c r="E98">
-        <v>6.2</v>
+        <v>0.8</v>
       </c>
       <c r="F98">
-        <v>27805</v>
+        <v>6601</v>
       </c>
       <c r="G98">
         <v>5</v>
       </c>
       <c r="H98">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I98">
-        <v>0</v>
+        <v>67</v>
       </c>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B99" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="C99" t="s">
-        <v>67</v>
+        <v>49</v>
       </c>
       <c r="D99">
-        <v>3621</v>
+        <v>1678</v>
       </c>
       <c r="E99">
-        <v>5.5</v>
+        <v>1.4</v>
       </c>
       <c r="F99">
-        <v>24668</v>
+        <v>11520</v>
       </c>
       <c r="G99">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H99">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I99">
-        <v>41072</v>
+        <v>51</v>
       </c>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>80</v>
+        <v>12</v>
       </c>
       <c r="B100" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C100" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D100">
-        <v>51</v>
+        <v>3931</v>
       </c>
       <c r="E100">
-        <v>0.7</v>
+        <v>6</v>
       </c>
       <c r="F100">
-        <v>22</v>
+        <v>26678</v>
       </c>
       <c r="G100">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="H100">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="I100">
-        <v>0</v>
+        <v>47765</v>
       </c>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>80</v>
+        <v>12</v>
       </c>
       <c r="B101" t="s">
+        <v>39</v>
+      </c>
+      <c r="C101" t="s">
         <v>38</v>
       </c>
-      <c r="C101" t="s">
-        <v>81</v>
-      </c>
       <c r="D101">
-        <v>556</v>
+        <v>3931</v>
       </c>
       <c r="E101">
-        <v>2.2000000000000002</v>
+        <v>6</v>
       </c>
       <c r="F101">
-        <v>64</v>
+        <v>26542</v>
       </c>
       <c r="G101">
+        <v>5</v>
+      </c>
+      <c r="H101">
         <v>2</v>
       </c>
-      <c r="H101">
-        <v>4</v>
-      </c>
       <c r="I101">
-        <v>172</v>
+        <v>46553</v>
       </c>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>80</v>
+        <v>12</v>
       </c>
       <c r="B102" t="s">
-        <v>81</v>
+        <v>38</v>
       </c>
       <c r="C102" t="s">
-        <v>76</v>
+        <v>40</v>
       </c>
       <c r="D102">
-        <v>565</v>
+        <v>4759</v>
       </c>
       <c r="E102">
-        <v>2.2999999999999998</v>
+        <v>7.1</v>
       </c>
       <c r="F102">
-        <v>61</v>
+        <v>31912</v>
       </c>
       <c r="G102">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H102">
         <v>4</v>
       </c>
       <c r="I102">
-        <v>172</v>
+        <v>40982</v>
       </c>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>80</v>
+        <v>12</v>
       </c>
       <c r="B103" t="s">
-        <v>76</v>
+        <v>40</v>
       </c>
       <c r="C103" t="s">
-        <v>96</v>
+        <v>38</v>
       </c>
       <c r="D103">
-        <v>931</v>
+        <v>4759</v>
       </c>
       <c r="E103">
-        <v>3.4</v>
+        <v>7.1</v>
       </c>
       <c r="F103">
-        <v>96</v>
+        <v>31601</v>
       </c>
       <c r="G103">
         <v>4</v>
       </c>
       <c r="H103">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I103">
-        <v>0</v>
+        <v>37607</v>
       </c>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>80</v>
+        <v>12</v>
       </c>
       <c r="B104" t="s">
-        <v>76</v>
+        <v>38</v>
       </c>
       <c r="C104" t="s">
-        <v>97</v>
+        <v>39</v>
       </c>
       <c r="D104">
-        <v>781</v>
+        <v>3931</v>
       </c>
       <c r="E104">
-        <v>2.9</v>
+        <v>6</v>
       </c>
       <c r="F104">
-        <v>83</v>
+        <v>26678</v>
       </c>
       <c r="G104">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H104">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I104">
-        <v>139</v>
+        <v>47765</v>
       </c>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>80</v>
+        <v>12</v>
       </c>
       <c r="B105" t="s">
-        <v>97</v>
+        <v>39</v>
       </c>
       <c r="C105" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D105">
-        <v>395</v>
+        <v>3931</v>
       </c>
       <c r="E105">
-        <v>1.7</v>
+        <v>6</v>
       </c>
       <c r="F105">
-        <v>61</v>
+        <v>26542</v>
       </c>
       <c r="G105">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H105">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="I105">
-        <v>139</v>
+        <v>46553</v>
       </c>
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B106" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C106" t="s">
-        <v>98</v>
+        <v>40</v>
       </c>
       <c r="D106">
-        <v>1752</v>
+        <v>4759</v>
       </c>
       <c r="E106">
-        <v>2.2999999999999998</v>
+        <v>7.1</v>
       </c>
       <c r="F106">
-        <v>860</v>
+        <v>31912</v>
       </c>
       <c r="G106">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="H106">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I106">
-        <v>0</v>
+        <v>40982</v>
       </c>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B107" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C107" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="D107">
-        <v>36</v>
+        <v>4759</v>
       </c>
       <c r="E107">
-        <v>0.5</v>
+        <v>7.1</v>
       </c>
       <c r="F107">
-        <v>230</v>
+        <v>31601</v>
       </c>
       <c r="G107">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H107">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I107">
-        <v>0</v>
+        <v>37607</v>
       </c>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
+        <v>12</v>
+      </c>
+      <c r="B108" t="s">
+        <v>38</v>
+      </c>
+      <c r="C108" t="s">
+        <v>60</v>
+      </c>
+      <c r="D108">
+        <v>2400</v>
+      </c>
+      <c r="E108">
+        <v>3.8</v>
+      </c>
+      <c r="F108">
+        <v>17325</v>
+      </c>
+      <c r="G108">
+        <v>2</v>
+      </c>
+      <c r="H108">
+        <v>3</v>
+      </c>
+      <c r="I108">
+        <v>47148</v>
+      </c>
+    </row>
+    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>12</v>
+      </c>
+      <c r="B109" t="s">
+        <v>60</v>
+      </c>
+      <c r="C109" t="s">
+        <v>61</v>
+      </c>
+      <c r="D109">
+        <v>2097</v>
+      </c>
+      <c r="E109">
+        <v>3.4</v>
+      </c>
+      <c r="F109">
+        <v>15401</v>
+      </c>
+      <c r="G109">
+        <v>3</v>
+      </c>
+      <c r="H109">
+        <v>2</v>
+      </c>
+      <c r="I109">
+        <v>48747</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>12</v>
+      </c>
+      <c r="B110" t="s">
+        <v>61</v>
+      </c>
+      <c r="C110" t="s">
+        <v>38</v>
+      </c>
+      <c r="D110">
+        <v>1186</v>
+      </c>
+      <c r="E110">
+        <v>2.1</v>
+      </c>
+      <c r="F110">
+        <v>9765</v>
+      </c>
+      <c r="G110">
+        <v>2</v>
+      </c>
+      <c r="H110">
+        <v>2</v>
+      </c>
+      <c r="I110">
+        <v>46386</v>
+      </c>
+    </row>
+    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>12</v>
+      </c>
+      <c r="B111" t="s">
+        <v>38</v>
+      </c>
+      <c r="C111" t="s">
+        <v>55</v>
+      </c>
+      <c r="D111">
+        <v>1950</v>
+      </c>
+      <c r="E111">
+        <v>3.2</v>
+      </c>
+      <c r="F111">
+        <v>14562</v>
+      </c>
+      <c r="G111">
+        <v>2</v>
+      </c>
+      <c r="H111">
+        <v>2</v>
+      </c>
+      <c r="I111">
+        <v>47462</v>
+      </c>
+    </row>
+    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>12</v>
+      </c>
+      <c r="B112" t="s">
+        <v>55</v>
+      </c>
+      <c r="C112" t="s">
+        <v>56</v>
+      </c>
+      <c r="D112">
+        <v>181</v>
+      </c>
+      <c r="E112">
+        <v>0.8</v>
+      </c>
+      <c r="F112">
+        <v>3666</v>
+      </c>
+      <c r="G112">
+        <v>2</v>
+      </c>
+      <c r="H112">
+        <v>4</v>
+      </c>
+      <c r="I112">
+        <v>43984</v>
+      </c>
+    </row>
+    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>12</v>
+      </c>
+      <c r="B113" t="s">
+        <v>56</v>
+      </c>
+      <c r="C113" t="s">
+        <v>38</v>
+      </c>
+      <c r="D113">
+        <v>1809</v>
+      </c>
+      <c r="E113">
+        <v>3</v>
+      </c>
+      <c r="F113">
+        <v>13568</v>
+      </c>
+      <c r="G113">
+        <v>4</v>
+      </c>
+      <c r="H113">
+        <v>2</v>
+      </c>
+      <c r="I113">
+        <v>41907</v>
+      </c>
+    </row>
+    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>12</v>
+      </c>
+      <c r="B114" t="s">
+        <v>38</v>
+      </c>
+      <c r="C114" t="s">
+        <v>57</v>
+      </c>
+      <c r="D114">
+        <v>796</v>
+      </c>
+      <c r="E114">
+        <v>1.6</v>
+      </c>
+      <c r="F114">
+        <v>7395</v>
+      </c>
+      <c r="G114">
+        <v>2</v>
+      </c>
+      <c r="H114">
+        <v>3</v>
+      </c>
+      <c r="I114">
+        <v>45199</v>
+      </c>
+    </row>
+    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>12</v>
+      </c>
+      <c r="B115" t="s">
+        <v>57</v>
+      </c>
+      <c r="C115" t="s">
+        <v>58</v>
+      </c>
+      <c r="D115">
+        <v>880</v>
+      </c>
+      <c r="E115">
+        <v>1.7</v>
+      </c>
+      <c r="F115">
+        <v>7927</v>
+      </c>
+      <c r="G115">
+        <v>3</v>
+      </c>
+      <c r="H115">
+        <v>2</v>
+      </c>
+      <c r="I115">
+        <v>43359</v>
+      </c>
+    </row>
+    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>12</v>
+      </c>
+      <c r="B116" t="s">
+        <v>58</v>
+      </c>
+      <c r="C116" t="s">
+        <v>59</v>
+      </c>
+      <c r="D116">
+        <v>200</v>
+      </c>
+      <c r="E116">
+        <v>0.8</v>
+      </c>
+      <c r="F116">
+        <v>3818</v>
+      </c>
+      <c r="G116">
+        <v>2</v>
+      </c>
+      <c r="H116">
+        <v>5</v>
+      </c>
+      <c r="I116">
+        <v>41287</v>
+      </c>
+    </row>
+    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>12</v>
+      </c>
+      <c r="B117" t="s">
+        <v>59</v>
+      </c>
+      <c r="C117" t="s">
+        <v>38</v>
+      </c>
+      <c r="D117">
+        <v>1504</v>
+      </c>
+      <c r="E117">
+        <v>2.6</v>
+      </c>
+      <c r="F117">
+        <v>11708</v>
+      </c>
+      <c r="G117">
+        <v>5</v>
+      </c>
+      <c r="H117">
+        <v>2</v>
+      </c>
+      <c r="I117">
+        <v>41972</v>
+      </c>
+    </row>
+    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>12</v>
+      </c>
+      <c r="B118" t="s">
+        <v>38</v>
+      </c>
+      <c r="C118" t="s">
+        <v>57</v>
+      </c>
+      <c r="D118">
+        <v>796</v>
+      </c>
+      <c r="E118">
+        <v>1.6</v>
+      </c>
+      <c r="F118">
+        <v>7395</v>
+      </c>
+      <c r="G118">
+        <v>2</v>
+      </c>
+      <c r="H118">
+        <v>3</v>
+      </c>
+      <c r="I118">
+        <v>45199</v>
+      </c>
+    </row>
+    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>12</v>
+      </c>
+      <c r="B119" t="s">
+        <v>57</v>
+      </c>
+      <c r="C119" t="s">
+        <v>58</v>
+      </c>
+      <c r="D119">
+        <v>880</v>
+      </c>
+      <c r="E119">
+        <v>1.7</v>
+      </c>
+      <c r="F119">
+        <v>7927</v>
+      </c>
+      <c r="G119">
+        <v>3</v>
+      </c>
+      <c r="H119">
+        <v>3</v>
+      </c>
+      <c r="I119">
+        <v>43359</v>
+      </c>
+    </row>
+    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>12</v>
+      </c>
+      <c r="B120" t="s">
+        <v>58</v>
+      </c>
+      <c r="C120" t="s">
+        <v>59</v>
+      </c>
+      <c r="D120">
+        <v>200</v>
+      </c>
+      <c r="E120">
+        <v>0.8</v>
+      </c>
+      <c r="F120">
+        <v>3818</v>
+      </c>
+      <c r="G120">
+        <v>3</v>
+      </c>
+      <c r="H120">
+        <v>5</v>
+      </c>
+      <c r="I120">
+        <v>41287</v>
+      </c>
+    </row>
+    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>12</v>
+      </c>
+      <c r="B121" t="s">
+        <v>59</v>
+      </c>
+      <c r="C121" t="s">
+        <v>38</v>
+      </c>
+      <c r="D121">
+        <v>1504</v>
+      </c>
+      <c r="E121">
+        <v>2.6</v>
+      </c>
+      <c r="F121">
+        <v>11708</v>
+      </c>
+      <c r="G121">
+        <v>5</v>
+      </c>
+      <c r="H121">
+        <v>2</v>
+      </c>
+      <c r="I121">
+        <v>41972</v>
+      </c>
+    </row>
+    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>12</v>
+      </c>
+      <c r="B122" t="s">
+        <v>38</v>
+      </c>
+      <c r="C122" t="s">
+        <v>65</v>
+      </c>
+      <c r="D122">
+        <v>2171</v>
+      </c>
+      <c r="E122">
+        <v>3.5</v>
+      </c>
+      <c r="F122">
+        <v>15594</v>
+      </c>
+      <c r="G122">
+        <v>2</v>
+      </c>
+      <c r="H122">
+        <v>5</v>
+      </c>
+      <c r="I122">
+        <v>6861</v>
+      </c>
+    </row>
+    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>12</v>
+      </c>
+      <c r="B123" t="s">
+        <v>65</v>
+      </c>
+      <c r="C123" t="s">
+        <v>66</v>
+      </c>
+      <c r="D123">
+        <v>4103</v>
+      </c>
+      <c r="E123">
+        <v>6.2</v>
+      </c>
+      <c r="F123">
+        <v>27805</v>
+      </c>
+      <c r="G123">
+        <v>5</v>
+      </c>
+      <c r="H123">
+        <v>5</v>
+      </c>
+      <c r="I123">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
+        <v>12</v>
+      </c>
+      <c r="B124" t="s">
+        <v>66</v>
+      </c>
+      <c r="C124" t="s">
+        <v>67</v>
+      </c>
+      <c r="D124">
+        <v>3621</v>
+      </c>
+      <c r="E124">
+        <v>5.5</v>
+      </c>
+      <c r="F124">
+        <v>24668</v>
+      </c>
+      <c r="G124">
+        <v>5</v>
+      </c>
+      <c r="H124">
+        <v>5</v>
+      </c>
+      <c r="I124">
+        <v>41072</v>
+      </c>
+    </row>
+    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>99</v>
+      </c>
+      <c r="B125" t="s">
+        <v>49</v>
+      </c>
+      <c r="C125" t="s">
+        <v>100</v>
+      </c>
+      <c r="D125">
+        <v>215</v>
+      </c>
+      <c r="E125">
+        <v>1.8</v>
+      </c>
+      <c r="F125">
+        <v>87</v>
+      </c>
+      <c r="G125">
+        <v>1</v>
+      </c>
+      <c r="H125">
+        <v>5</v>
+      </c>
+      <c r="I125">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
+        <v>99</v>
+      </c>
+      <c r="B126" t="s">
+        <v>100</v>
+      </c>
+      <c r="C126" t="s">
+        <v>101</v>
+      </c>
+      <c r="D126">
+        <v>362</v>
+      </c>
+      <c r="E126">
+        <v>2.8</v>
+      </c>
+      <c r="F126">
+        <v>115</v>
+      </c>
+      <c r="G126">
+        <v>5</v>
+      </c>
+      <c r="H126">
+        <v>4</v>
+      </c>
+      <c r="I126">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
+        <v>99</v>
+      </c>
+      <c r="B127" t="s">
+        <v>101</v>
+      </c>
+      <c r="C127" t="s">
+        <v>49</v>
+      </c>
+      <c r="D127">
+        <v>192</v>
+      </c>
+      <c r="E127">
+        <v>1.7</v>
+      </c>
+      <c r="F127">
+        <v>87</v>
+      </c>
+      <c r="G127">
+        <v>4</v>
+      </c>
+      <c r="H127">
+        <v>1</v>
+      </c>
+      <c r="I127">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
+        <v>99</v>
+      </c>
+      <c r="B128" t="s">
+        <v>49</v>
+      </c>
+      <c r="C128" t="s">
+        <v>102</v>
+      </c>
+      <c r="D128">
+        <v>183</v>
+      </c>
+      <c r="E128">
+        <v>1.6</v>
+      </c>
+      <c r="F128">
+        <v>79</v>
+      </c>
+      <c r="G128">
+        <v>1</v>
+      </c>
+      <c r="H128">
+        <v>4</v>
+      </c>
+      <c r="I128">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
+        <v>99</v>
+      </c>
+      <c r="B129" t="s">
+        <v>102</v>
+      </c>
+      <c r="C129" t="s">
+        <v>100</v>
+      </c>
+      <c r="D129">
+        <v>395</v>
+      </c>
+      <c r="E129">
+        <v>3</v>
+      </c>
+      <c r="F129">
+        <v>131</v>
+      </c>
+      <c r="G129">
+        <v>4</v>
+      </c>
+      <c r="H129">
+        <v>5</v>
+      </c>
+      <c r="I129">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
+        <v>99</v>
+      </c>
+      <c r="B130" t="s">
+        <v>100</v>
+      </c>
+      <c r="C130" t="s">
+        <v>49</v>
+      </c>
+      <c r="D130">
+        <v>215</v>
+      </c>
+      <c r="E130">
+        <v>1.8</v>
+      </c>
+      <c r="F130">
+        <v>92</v>
+      </c>
+      <c r="G130">
+        <v>5</v>
+      </c>
+      <c r="H130">
+        <v>1</v>
+      </c>
+      <c r="I130">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
+        <v>99</v>
+      </c>
+      <c r="B131" t="s">
+        <v>49</v>
+      </c>
+      <c r="C131" t="s">
+        <v>103</v>
+      </c>
+      <c r="D131">
+        <v>410</v>
+      </c>
+      <c r="E131">
+        <v>3.1</v>
+      </c>
+      <c r="F131">
+        <v>137</v>
+      </c>
+      <c r="G131">
+        <v>1</v>
+      </c>
+      <c r="H131">
+        <v>4</v>
+      </c>
+      <c r="I131">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="132" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
+        <v>99</v>
+      </c>
+      <c r="B132" t="s">
+        <v>103</v>
+      </c>
+      <c r="C132" t="s">
+        <v>104</v>
+      </c>
+      <c r="D132">
+        <v>207</v>
+      </c>
+      <c r="E132">
+        <v>1.8</v>
+      </c>
+      <c r="F132">
+        <v>72</v>
+      </c>
+      <c r="G132">
+        <v>4</v>
+      </c>
+      <c r="H132">
+        <v>4</v>
+      </c>
+      <c r="I132">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
+        <v>99</v>
+      </c>
+      <c r="B133" t="s">
+        <v>104</v>
+      </c>
+      <c r="C133" t="s">
+        <v>49</v>
+      </c>
+      <c r="D133">
+        <v>325</v>
+      </c>
+      <c r="E133">
+        <v>2.5</v>
+      </c>
+      <c r="F133">
+        <v>120</v>
+      </c>
+      <c r="G133">
+        <v>4</v>
+      </c>
+      <c r="H133">
+        <v>1</v>
+      </c>
+      <c r="I133">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="134" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
+        <v>99</v>
+      </c>
+      <c r="B134" t="s">
+        <v>49</v>
+      </c>
+      <c r="C134" t="s">
+        <v>102</v>
+      </c>
+      <c r="D134">
+        <v>183</v>
+      </c>
+      <c r="E134">
+        <v>1.6</v>
+      </c>
+      <c r="F134">
+        <v>79</v>
+      </c>
+      <c r="G134">
+        <v>1</v>
+      </c>
+      <c r="H134">
+        <v>4</v>
+      </c>
+      <c r="I134">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="135" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
+        <v>99</v>
+      </c>
+      <c r="B135" t="s">
+        <v>102</v>
+      </c>
+      <c r="C135" t="s">
+        <v>49</v>
+      </c>
+      <c r="D135">
+        <v>183</v>
+      </c>
+      <c r="E135">
+        <v>1.6</v>
+      </c>
+      <c r="F135">
+        <v>85</v>
+      </c>
+      <c r="G135">
+        <v>4</v>
+      </c>
+      <c r="H135">
+        <v>1</v>
+      </c>
+      <c r="I135">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
+        <v>99</v>
+      </c>
+      <c r="B136" t="s">
+        <v>49</v>
+      </c>
+      <c r="C136" t="s">
+        <v>105</v>
+      </c>
+      <c r="D136">
+        <v>89</v>
+      </c>
+      <c r="E136">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F136">
+        <v>91</v>
+      </c>
+      <c r="G136">
+        <v>1</v>
+      </c>
+      <c r="H136">
+        <v>5</v>
+      </c>
+      <c r="I136">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="137" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
+        <v>99</v>
+      </c>
+      <c r="B137" t="s">
+        <v>105</v>
+      </c>
+      <c r="C137" t="s">
+        <v>49</v>
+      </c>
+      <c r="D137">
+        <v>89</v>
+      </c>
+      <c r="E137">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F137">
+        <v>62</v>
+      </c>
+      <c r="G137">
+        <v>5</v>
+      </c>
+      <c r="H137">
+        <v>1</v>
+      </c>
+      <c r="I137">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="138" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
+        <v>99</v>
+      </c>
+      <c r="B138" t="s">
+        <v>49</v>
+      </c>
+      <c r="C138" t="s">
+        <v>106</v>
+      </c>
+      <c r="D138">
+        <v>147</v>
+      </c>
+      <c r="E138">
+        <v>1.4</v>
+      </c>
+      <c r="F138">
+        <v>70</v>
+      </c>
+      <c r="G138">
+        <v>1</v>
+      </c>
+      <c r="H138">
+        <v>4</v>
+      </c>
+      <c r="I138">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="139" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
+        <v>99</v>
+      </c>
+      <c r="B139" t="s">
+        <v>106</v>
+      </c>
+      <c r="C139" t="s">
+        <v>49</v>
+      </c>
+      <c r="D139">
+        <v>147</v>
+      </c>
+      <c r="E139">
+        <v>1.4</v>
+      </c>
+      <c r="F139">
+        <v>76</v>
+      </c>
+      <c r="G139">
+        <v>4</v>
+      </c>
+      <c r="H139">
+        <v>1</v>
+      </c>
+      <c r="I139">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="140" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
+        <v>99</v>
+      </c>
+      <c r="B140" t="s">
+        <v>49</v>
+      </c>
+      <c r="C140" t="s">
+        <v>69</v>
+      </c>
+      <c r="D140">
+        <v>257</v>
+      </c>
+      <c r="E140">
+        <v>2.1</v>
+      </c>
+      <c r="F140">
+        <v>98</v>
+      </c>
+      <c r="G140">
+        <v>1</v>
+      </c>
+      <c r="H140">
+        <v>5</v>
+      </c>
+      <c r="I140">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="141" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A141" t="s">
+        <v>99</v>
+      </c>
+      <c r="B141" t="s">
+        <v>69</v>
+      </c>
+      <c r="C141" t="s">
+        <v>41</v>
+      </c>
+      <c r="D141">
+        <v>225</v>
+      </c>
+      <c r="E141">
+        <v>1.9</v>
+      </c>
+      <c r="F141">
+        <v>118</v>
+      </c>
+      <c r="G141">
+        <v>5</v>
+      </c>
+      <c r="H141">
+        <v>5</v>
+      </c>
+      <c r="I141">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="142" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A142" t="s">
+        <v>99</v>
+      </c>
+      <c r="B142" t="s">
+        <v>41</v>
+      </c>
+      <c r="C142" t="s">
+        <v>49</v>
+      </c>
+      <c r="D142">
+        <v>36</v>
+      </c>
+      <c r="E142">
+        <v>0.7</v>
+      </c>
+      <c r="F142">
+        <v>49</v>
+      </c>
+      <c r="G142">
+        <v>5</v>
+      </c>
+      <c r="H142">
+        <v>1</v>
+      </c>
+      <c r="I142">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="143" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
+        <v>80</v>
+      </c>
+      <c r="B143" t="s">
+        <v>41</v>
+      </c>
+      <c r="C143" t="s">
+        <v>38</v>
+      </c>
+      <c r="D143">
+        <v>51</v>
+      </c>
+      <c r="E143">
+        <v>0.7</v>
+      </c>
+      <c r="F143">
+        <v>22</v>
+      </c>
+      <c r="G143">
+        <v>5</v>
+      </c>
+      <c r="H143">
+        <v>2</v>
+      </c>
+      <c r="I143">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="144" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
+        <v>80</v>
+      </c>
+      <c r="B144" t="s">
+        <v>38</v>
+      </c>
+      <c r="C144" t="s">
+        <v>81</v>
+      </c>
+      <c r="D144">
+        <v>556</v>
+      </c>
+      <c r="E144">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="F144">
+        <v>64</v>
+      </c>
+      <c r="G144">
+        <v>2</v>
+      </c>
+      <c r="H144">
+        <v>4</v>
+      </c>
+      <c r="I144">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="145" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
+        <v>80</v>
+      </c>
+      <c r="B145" t="s">
+        <v>81</v>
+      </c>
+      <c r="C145" t="s">
+        <v>76</v>
+      </c>
+      <c r="D145">
+        <v>565</v>
+      </c>
+      <c r="E145">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="F145">
+        <v>61</v>
+      </c>
+      <c r="G145">
+        <v>4</v>
+      </c>
+      <c r="H145">
+        <v>4</v>
+      </c>
+      <c r="I145">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="146" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
+        <v>80</v>
+      </c>
+      <c r="B146" t="s">
+        <v>76</v>
+      </c>
+      <c r="C146" t="s">
+        <v>96</v>
+      </c>
+      <c r="D146">
+        <v>931</v>
+      </c>
+      <c r="E146">
+        <v>3.4</v>
+      </c>
+      <c r="F146">
+        <v>96</v>
+      </c>
+      <c r="G146">
+        <v>4</v>
+      </c>
+      <c r="H146">
+        <v>4</v>
+      </c>
+      <c r="I146">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="147" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
+        <v>80</v>
+      </c>
+      <c r="B147" t="s">
+        <v>76</v>
+      </c>
+      <c r="C147" t="s">
+        <v>97</v>
+      </c>
+      <c r="D147">
+        <v>781</v>
+      </c>
+      <c r="E147">
+        <v>2.9</v>
+      </c>
+      <c r="F147">
+        <v>83</v>
+      </c>
+      <c r="G147">
+        <v>4</v>
+      </c>
+      <c r="H147">
+        <v>4</v>
+      </c>
+      <c r="I147">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="148" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
+        <v>80</v>
+      </c>
+      <c r="B148" t="s">
+        <v>97</v>
+      </c>
+      <c r="C148" t="s">
+        <v>41</v>
+      </c>
+      <c r="D148">
+        <v>395</v>
+      </c>
+      <c r="E148">
+        <v>1.7</v>
+      </c>
+      <c r="F148">
+        <v>61</v>
+      </c>
+      <c r="G148">
+        <v>4</v>
+      </c>
+      <c r="H148">
+        <v>5</v>
+      </c>
+      <c r="I148">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="149" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
         <v>14</v>
       </c>
-      <c r="B108" t="s">
+      <c r="B149" t="s">
         <v>41</v>
       </c>
-      <c r="C108" t="s">
+      <c r="C149" t="s">
+        <v>98</v>
+      </c>
+      <c r="D149">
+        <v>1752</v>
+      </c>
+      <c r="E149">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="F149">
+        <v>860</v>
+      </c>
+      <c r="G149">
+        <v>5</v>
+      </c>
+      <c r="H149">
+        <v>5</v>
+      </c>
+      <c r="I149">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="150" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A150" t="s">
+        <v>14</v>
+      </c>
+      <c r="B150" t="s">
+        <v>41</v>
+      </c>
+      <c r="C150" t="s">
+        <v>49</v>
+      </c>
+      <c r="D150">
+        <v>36</v>
+      </c>
+      <c r="E150">
+        <v>0.5</v>
+      </c>
+      <c r="F150">
+        <v>230</v>
+      </c>
+      <c r="G150">
+        <v>5</v>
+      </c>
+      <c r="H150">
+        <v>1</v>
+      </c>
+      <c r="I150">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="151" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A151" t="s">
+        <v>14</v>
+      </c>
+      <c r="B151" t="s">
+        <v>41</v>
+      </c>
+      <c r="C151" t="s">
         <v>73</v>
       </c>
-      <c r="D108">
+      <c r="D151">
         <v>742</v>
       </c>
-      <c r="E108">
+      <c r="E151">
         <v>1.2</v>
       </c>
-      <c r="F108">
+      <c r="F151">
         <v>484</v>
       </c>
-      <c r="G108">
-        <v>5</v>
-      </c>
-      <c r="H108">
-        <v>5</v>
-      </c>
-      <c r="I108">
+      <c r="G151">
+        <v>5</v>
+      </c>
+      <c r="H151">
+        <v>5</v>
+      </c>
+      <c r="I151">
         <v>8355</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I102">
-    <sortCondition ref="A2:A102"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I151">
+    <sortCondition ref="A2:A151"/>
   </sortState>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>